<commit_message>
Added Course Materials - Day 4.
</commit_message>
<xml_diff>
--- a/JEE DevOps - TOC.xlsx
+++ b/JEE DevOps - TOC.xlsx
@@ -4,22 +4,23 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20490" windowHeight="7815" activeTab="5"/>
+    <workbookView windowWidth="20490" windowHeight="7815" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="7" r:id="rId1"/>
-    <sheet name="Spring Core" sheetId="13" r:id="rId2"/>
-    <sheet name="Spring MVC" sheetId="14" r:id="rId3"/>
-    <sheet name="Spring REST" sheetId="15" r:id="rId4"/>
-    <sheet name="Spring  Data JPA" sheetId="16" r:id="rId5"/>
-    <sheet name="Spring Data REST" sheetId="17" r:id="rId6"/>
+    <sheet name="JPA with Hibernate" sheetId="10" r:id="rId2"/>
+    <sheet name="Spring Core" sheetId="13" r:id="rId3"/>
+    <sheet name="Spring MVC" sheetId="14" r:id="rId4"/>
+    <sheet name="Spring REST" sheetId="15" r:id="rId5"/>
+    <sheet name="Spring  Data JPA" sheetId="16" r:id="rId6"/>
+    <sheet name="Spring Data REST" sheetId="17" r:id="rId7"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="386" uniqueCount="316">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="443" uniqueCount="367">
   <si>
     <t>Sr. No.</t>
   </si>
@@ -75,15 +76,223 @@
     <t>Sections</t>
   </si>
   <si>
+    <t>Day 1</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Learn to interact with database applications from Java programs using the Hibernate framework.                       </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Explore object-relational mapping (ORM) and its problems.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">                           </t>
+    </r>
+  </si>
+  <si>
+    <t>1. Course Overview</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2. Introducing ORM and Its Problems </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Introducing ORM and Its Problems </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2. The Granularity Problem </t>
+  </si>
+  <si>
+    <t xml:space="preserve">3. The Inheritance Problem </t>
+  </si>
+  <si>
+    <t xml:space="preserve">5. The Associations Problem </t>
+  </si>
+  <si>
+    <t xml:space="preserve">6. The Data Navigation Problem </t>
+  </si>
+  <si>
+    <t>7. A Simple Hibernate Application</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3. Working with Entities </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Introducing Working with Entities </t>
+  </si>
+  <si>
+    <t>2. Demo: A Secondary Table with One Field</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3. Demo: A Secondary Table with Multiple Fields </t>
+  </si>
+  <si>
+    <t xml:space="preserve">4. Demo: Multiple Secondary Tables </t>
+  </si>
+  <si>
+    <t xml:space="preserve">5. Entity Access Types </t>
+  </si>
+  <si>
+    <t xml:space="preserve">6. Entity Primary Keys and Entity Identity  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">7. Demo: Primary Keys with @GeneratedValue </t>
+  </si>
+  <si>
+    <t xml:space="preserve">8. Demo: Embeddable Primary Key and Embedded ID </t>
+  </si>
+  <si>
+    <t xml:space="preserve">9. Demo: Embeddable Primary Key and ID Class </t>
+  </si>
+  <si>
+    <t>Day 2</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Discover entities, entity relationships, and inheritance.                </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Work with the EntityManager API.                                When you’re finished with this course, you’ll have the skills and knowledge needed to quickly and efficiently develop Java database applications using Hibernate.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">4. Entity Relationships </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Introducing Entity Relationships </t>
+  </si>
+  <si>
+    <t>2. Demo: Define One-to-many and Many-to-one Relationships</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3. Demo: Define Many-to-many Relationships  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">4.Annotations for Relationship Definition </t>
+  </si>
+  <si>
+    <t xml:space="preserve">5. Demo: Join Tables on One Column </t>
+  </si>
+  <si>
+    <t xml:space="preserve">6. Demo: Join Tables on Multiple Columns </t>
+  </si>
+  <si>
+    <t xml:space="preserve">7. Embeddable Classes </t>
+  </si>
+  <si>
+    <t>8. Demo: Embedding Classes in Entities</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9. Demo: Embedding Collections of Classes in Entities </t>
+  </si>
+  <si>
+    <t>10. Demo: Embedding Maps of Classes in Entities</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5. Entity Inheritance  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Introducing Entity Inheritance </t>
+  </si>
+  <si>
+    <t>2. Demo: Extend One Entity</t>
+  </si>
+  <si>
+    <t>3. Demo: Extend One Non-entity</t>
+  </si>
+  <si>
+    <t>4. Mapping Strategies</t>
+  </si>
+  <si>
+    <t>5. Demo: Single Table per Class Hierarchy</t>
+  </si>
+  <si>
+    <t>6. Demo: Joined Subclass Strategy</t>
+  </si>
+  <si>
+    <t>7. Demo: Table per Concrete Class Strategy</t>
+  </si>
+  <si>
+    <t>8. Demo: Conversion</t>
+  </si>
+  <si>
+    <t>6. The EntityManager API</t>
+  </si>
+  <si>
+    <t>1. Introducing the EntityManager API</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2. Demo: Application-managed EntityManager </t>
+  </si>
+  <si>
+    <t>3. Demo: Container-managed EntityManager</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4. Finding Entities Using the EntityManager
+</t>
+  </si>
+  <si>
+    <t>5. Conclusions</t>
+  </si>
+  <si>
+    <t>Hands On Assignments</t>
+  </si>
+  <si>
+    <t>JPA Using Hibernate And  PostgreSQL</t>
+  </si>
+  <si>
+    <t>jpa-hibernate-exercises.zip</t>
+  </si>
+  <si>
+    <t>Total # of Days for JPA with Hibernate</t>
+  </si>
+  <si>
+    <t>Total # of Hours for JPA with Hibernate</t>
+  </si>
+  <si>
     <t>Day 3</t>
   </si>
   <si>
     <t>Spring Framework:                           Spring Fundamentals</t>
   </si>
   <si>
-    <t>1. Course Overview</t>
-  </si>
-  <si>
     <t>2. What Is Spring?</t>
   </si>
   <si>
@@ -253,9 +462,6 @@
   </si>
   <si>
     <t>8. Summary</t>
-  </si>
-  <si>
-    <t>Hands On Assignments</t>
   </si>
   <si>
     <t>Spring Framework : Spring Fundamentals</t>
@@ -1037,8 +1243,8 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="38">
@@ -1174,9 +1380,16 @@
       <charset val="134"/>
     </font>
     <font>
-      <u/>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1190,14 +1403,44 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1213,7 +1456,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1232,20 +1475,6 @@
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1282,35 +1511,12 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -1351,7 +1557,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1363,91 +1593,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1465,7 +1617,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1477,7 +1635,73 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1489,49 +1713,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1628,19 +1834,38 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
       <top style="thin">
-        <color theme="4"/>
+        <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1684,17 +1909,13 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
+      <left/>
+      <right/>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color theme="4"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1702,30 +1923,15 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="22" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1743,134 +1949,134 @@
     <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="19" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="12" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="15" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="12" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="14" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="11" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="29" fillId="14" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="24" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="36" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="23" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="23" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1943,6 +2149,18 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2312,7 +2530,7 @@
   <sheetPr/>
   <dimension ref="A7:I22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
@@ -2326,137 +2544,137 @@
   <sheetData>
     <row r="7" ht="13.5"/>
     <row r="8" ht="13.5" spans="6:9">
-      <c r="F8" s="29" t="s">
+      <c r="F8" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="G8" s="30" t="s">
+      <c r="G8" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="H8" s="30" t="s">
+      <c r="H8" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="I8" s="30" t="s">
+      <c r="I8" s="34" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="9" ht="15.75" spans="6:9">
-      <c r="F9" s="31">
+      <c r="F9" s="35">
         <v>1</v>
       </c>
-      <c r="G9" s="32" t="s">
+      <c r="G9" s="36" t="s">
         <v>4</v>
       </c>
-      <c r="H9" s="33">
+      <c r="H9" s="37">
         <v>2</v>
       </c>
-      <c r="I9" s="33">
+      <c r="I9" s="37">
         <v>16</v>
       </c>
     </row>
     <row r="10" ht="15.75" spans="6:9">
-      <c r="F10" s="34">
+      <c r="F10" s="38">
         <v>2</v>
       </c>
-      <c r="G10" s="35" t="s">
+      <c r="G10" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="H10" s="33">
+      <c r="H10" s="37">
         <v>7</v>
       </c>
-      <c r="I10" s="33">
+      <c r="I10" s="37">
         <v>56</v>
       </c>
     </row>
     <row r="11" ht="14" customHeight="1" spans="6:9">
-      <c r="F11" s="36">
+      <c r="F11" s="40">
         <v>3</v>
       </c>
-      <c r="G11" s="35" t="s">
+      <c r="G11" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="H11" s="33">
+      <c r="H11" s="37">
         <v>2</v>
       </c>
-      <c r="I11" s="33">
+      <c r="I11" s="37">
         <v>16</v>
       </c>
     </row>
     <row r="12" ht="45.75" spans="6:9">
-      <c r="F12" s="34">
+      <c r="F12" s="38">
         <v>4</v>
       </c>
-      <c r="G12" s="32" t="s">
+      <c r="G12" s="36" t="s">
         <v>7</v>
       </c>
-      <c r="H12" s="33">
+      <c r="H12" s="37">
         <v>5</v>
       </c>
-      <c r="I12" s="33">
+      <c r="I12" s="37">
         <v>40</v>
       </c>
     </row>
     <row r="13" ht="15.75" spans="6:9">
-      <c r="F13" s="34">
+      <c r="F13" s="38">
         <v>5</v>
       </c>
-      <c r="G13" s="32" t="s">
+      <c r="G13" s="36" t="s">
         <v>8</v>
       </c>
-      <c r="H13" s="33">
+      <c r="H13" s="37">
         <v>1</v>
       </c>
-      <c r="I13" s="33">
+      <c r="I13" s="37">
         <v>8</v>
       </c>
     </row>
     <row r="14" ht="15.75" spans="6:9">
-      <c r="F14" s="37"/>
-      <c r="G14" s="38" t="s">
+      <c r="F14" s="41"/>
+      <c r="G14" s="42" t="s">
         <v>9</v>
       </c>
-      <c r="H14" s="39" t="s">
+      <c r="H14" s="43" t="s">
         <v>10</v>
       </c>
-      <c r="I14" s="39" t="s">
+      <c r="I14" s="43" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="19" spans="1:1">
-      <c r="A19" s="40" t="s">
+      <c r="A19" s="44" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="20" spans="1:6">
-      <c r="A20" s="41">
+      <c r="A20" s="45">
         <v>1</v>
       </c>
-      <c r="B20" s="42" t="s">
+      <c r="B20" s="46" t="s">
         <v>13</v>
       </c>
-      <c r="C20" s="42"/>
-      <c r="D20" s="42"/>
-      <c r="E20" s="42"/>
-      <c r="F20" s="42"/>
+      <c r="C20" s="46"/>
+      <c r="D20" s="46"/>
+      <c r="E20" s="46"/>
+      <c r="F20" s="46"/>
     </row>
     <row r="21" spans="1:6">
-      <c r="A21" s="41">
+      <c r="A21" s="45">
         <v>2</v>
       </c>
-      <c r="B21" s="43" t="s">
+      <c r="B21" s="47" t="s">
         <v>14</v>
       </c>
-      <c r="C21" s="43"/>
-      <c r="D21" s="43"/>
-      <c r="E21" s="43"/>
-      <c r="F21" s="43"/>
+      <c r="C21" s="47"/>
+      <c r="D21" s="47"/>
+      <c r="E21" s="47"/>
+      <c r="F21" s="47"/>
     </row>
     <row r="22" ht="26" customHeight="1" spans="1:6">
-      <c r="A22" s="44"/>
-      <c r="B22" s="45"/>
-      <c r="C22" s="45"/>
-      <c r="D22" s="45"/>
-      <c r="E22" s="45"/>
-      <c r="F22" s="45"/>
+      <c r="A22" s="48"/>
+      <c r="B22" s="49"/>
+      <c r="C22" s="49"/>
+      <c r="D22" s="49"/>
+      <c r="E22" s="49"/>
+      <c r="F22" s="49"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -2472,12 +2690,425 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
+  <dimension ref="A1:C55"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A34" activePane="bottomLeft" state="frozen"/>
+      <selection/>
+      <selection pane="bottomLeft" activeCell="C45" sqref="C45"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" outlineLevelCol="2"/>
+  <cols>
+    <col min="1" max="1" width="38.625" customWidth="1"/>
+    <col min="2" max="2" width="35.125" customWidth="1"/>
+    <col min="3" max="3" width="51.125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="16.5" spans="1:3">
+      <c r="A1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" ht="24.75" spans="1:3">
+      <c r="A2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+    </row>
+    <row r="3" ht="15.75" spans="1:3">
+      <c r="A3" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" s="29" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" ht="10" customHeight="1" spans="1:3">
+      <c r="A4" s="3"/>
+      <c r="B4" s="30"/>
+      <c r="C4" s="30"/>
+    </row>
+    <row r="5" ht="19" customHeight="1" spans="1:3">
+      <c r="A5" s="3"/>
+      <c r="B5" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" s="29" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="3"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" ht="18" customHeight="1" spans="1:3">
+      <c r="A7" s="3"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="31" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" ht="12" customHeight="1" spans="1:3">
+      <c r="A8" s="3"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="31" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" ht="15" spans="1:3">
+      <c r="A9" s="3"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="31" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" ht="15" spans="1:3">
+      <c r="A10" s="3"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" ht="14" customHeight="1" spans="1:3">
+      <c r="A11" s="3"/>
+      <c r="B11" s="4"/>
+      <c r="C11" s="5"/>
+    </row>
+    <row r="12" ht="52" customHeight="1" spans="1:3">
+      <c r="A12" s="3"/>
+      <c r="B12" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C12" s="31" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" ht="12" customHeight="1" spans="1:3">
+      <c r="A13" s="3"/>
+      <c r="B13" s="7"/>
+      <c r="C13" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" ht="24" customHeight="1" spans="1:3">
+      <c r="A14" s="3"/>
+      <c r="B14" s="7"/>
+      <c r="C14" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="15" ht="18" customHeight="1" spans="1:3">
+      <c r="A15" s="3"/>
+      <c r="B15" s="7"/>
+      <c r="C15" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="16" ht="15" spans="1:3">
+      <c r="A16" s="3"/>
+      <c r="B16" s="7"/>
+      <c r="C16" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="17" ht="15" spans="1:3">
+      <c r="A17" s="3"/>
+      <c r="B17" s="7"/>
+      <c r="C17" s="5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="18" ht="22" customHeight="1" spans="1:3">
+      <c r="A18" s="3"/>
+      <c r="B18" s="7"/>
+      <c r="C18" s="31" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="19" ht="18" customHeight="1" spans="1:3">
+      <c r="A19" s="3"/>
+      <c r="B19" s="7"/>
+      <c r="C19" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="20" ht="15" spans="1:3">
+      <c r="A20" s="3"/>
+      <c r="B20" s="7"/>
+      <c r="C20" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="21" ht="9" customHeight="1" spans="1:3">
+      <c r="A21" s="28"/>
+      <c r="B21" s="28"/>
+      <c r="C21" s="28"/>
+    </row>
+    <row r="22" ht="24.75" spans="1:3">
+      <c r="A22" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B22" s="2"/>
+      <c r="C22" s="2"/>
+    </row>
+    <row r="23" ht="38" customHeight="1" spans="1:3">
+      <c r="A23" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C23" s="31" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="24" ht="20" customHeight="1" spans="1:3">
+      <c r="A24" s="3"/>
+      <c r="B24" s="7"/>
+      <c r="C24" s="5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="25" ht="15" spans="1:3">
+      <c r="A25" s="3"/>
+      <c r="B25" s="7"/>
+      <c r="C25" s="5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="26" ht="21" customHeight="1" spans="1:3">
+      <c r="A26" s="3"/>
+      <c r="B26" s="7"/>
+      <c r="C26" s="31" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="27" ht="20" customHeight="1" spans="1:3">
+      <c r="A27" s="3"/>
+      <c r="B27" s="7"/>
+      <c r="C27" s="8" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="28" ht="15" spans="1:3">
+      <c r="A28" s="3"/>
+      <c r="B28" s="7"/>
+      <c r="C28" s="31" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="29" ht="17" customHeight="1" spans="1:3">
+      <c r="A29" s="3"/>
+      <c r="B29" s="7"/>
+      <c r="C29" s="5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="30" ht="13" customHeight="1" spans="1:3">
+      <c r="A30" s="3"/>
+      <c r="B30" s="7"/>
+      <c r="C30" s="5" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="31" ht="21" customHeight="1" spans="1:3">
+      <c r="A31" s="3"/>
+      <c r="B31" s="7"/>
+      <c r="C31" s="31" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
+      <c r="A32" s="3"/>
+      <c r="B32" s="7"/>
+      <c r="C32" s="32" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="33" ht="15.75" spans="1:3">
+      <c r="A33" s="3"/>
+      <c r="B33" s="7"/>
+      <c r="C33" s="32"/>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34" s="3"/>
+      <c r="B34" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="C34" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35" s="3"/>
+      <c r="B35" s="7"/>
+      <c r="C35" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36" s="3"/>
+      <c r="B36" s="7"/>
+      <c r="C36" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
+      <c r="A37" s="3"/>
+      <c r="B37" s="7"/>
+      <c r="C37" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3">
+      <c r="A38" s="3"/>
+      <c r="B38" s="7"/>
+      <c r="C38" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3">
+      <c r="A39" s="3"/>
+      <c r="B39" s="7"/>
+      <c r="C39" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3">
+      <c r="A40" s="3"/>
+      <c r="B40" s="7"/>
+      <c r="C40" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3">
+      <c r="A41" s="3"/>
+      <c r="B41" s="7"/>
+      <c r="C41" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1">
+      <c r="A42" s="3"/>
+    </row>
+    <row r="43" ht="18" customHeight="1" spans="1:3">
+      <c r="A43" s="3"/>
+      <c r="B43" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="C43" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="44" ht="18" customHeight="1" spans="1:3">
+      <c r="A44" s="3"/>
+      <c r="B44" s="7"/>
+      <c r="C44" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="45" ht="18" customHeight="1" spans="1:3">
+      <c r="A45" s="3"/>
+      <c r="B45" s="7"/>
+      <c r="C45" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="46" ht="16" customHeight="1" spans="1:3">
+      <c r="A46" s="3"/>
+      <c r="B46" s="7"/>
+      <c r="C46" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="47" ht="16" customHeight="1" spans="1:3">
+      <c r="A47" s="3"/>
+      <c r="B47" s="7"/>
+      <c r="C47" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1">
+      <c r="A48" s="3"/>
+    </row>
+    <row r="49" ht="15" spans="1:3">
+      <c r="A49" s="3"/>
+      <c r="B49" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="C49" s="10" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="50" ht="15" spans="1:3">
+      <c r="A50" s="3"/>
+      <c r="B50" s="9"/>
+      <c r="C50" s="5" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="51" ht="9" customHeight="1" spans="1:3">
+      <c r="A51" s="27"/>
+      <c r="B51" s="28"/>
+      <c r="C51" s="28"/>
+    </row>
+    <row r="54" ht="18.75" spans="1:2">
+      <c r="A54" s="19" t="s">
+        <v>69</v>
+      </c>
+      <c r="B54" s="20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="55" ht="18.75" spans="1:2">
+      <c r="A55" s="19" t="s">
+        <v>70</v>
+      </c>
+      <c r="B55" s="20">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="10">
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A22:C22"/>
+    <mergeCell ref="A3:A20"/>
+    <mergeCell ref="A23:A50"/>
+    <mergeCell ref="B5:B10"/>
+    <mergeCell ref="B12:B20"/>
+    <mergeCell ref="B23:B32"/>
+    <mergeCell ref="B34:B41"/>
+    <mergeCell ref="B43:B47"/>
+    <mergeCell ref="B49:B50"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:C78"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="A77" sqref="A77:B78"/>
+      <selection pane="bottomLeft" activeCell="A74" sqref="$A74:$XFD74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" outlineLevelCol="2"/>
@@ -2500,14 +3131,14 @@
     </row>
     <row r="2" ht="24.75" spans="1:3">
       <c r="A2" s="2" t="s">
-        <v>18</v>
+        <v>71</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
     </row>
     <row r="3" ht="15.75" spans="1:3">
       <c r="A3" s="25" t="s">
-        <v>19</v>
+        <v>72</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>20</v>
@@ -2524,73 +3155,73 @@
     <row r="5" ht="15" spans="1:3">
       <c r="A5" s="25"/>
       <c r="B5" s="7" t="s">
-        <v>21</v>
+        <v>73</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>22</v>
+        <v>74</v>
       </c>
     </row>
     <row r="6" ht="15" spans="1:3">
       <c r="A6" s="25"/>
       <c r="B6" s="7"/>
       <c r="C6" s="5" t="s">
-        <v>21</v>
+        <v>73</v>
       </c>
     </row>
     <row r="7" ht="15" spans="1:3">
       <c r="A7" s="25"/>
       <c r="B7" s="7"/>
       <c r="C7" s="5" t="s">
-        <v>23</v>
+        <v>75</v>
       </c>
     </row>
     <row r="8" ht="15" spans="1:3">
       <c r="A8" s="25"/>
       <c r="B8" s="7"/>
       <c r="C8" s="5" t="s">
-        <v>24</v>
+        <v>76</v>
       </c>
     </row>
     <row r="9" ht="15" spans="1:3">
       <c r="A9" s="25"/>
       <c r="B9" s="7"/>
       <c r="C9" s="5" t="s">
-        <v>25</v>
+        <v>77</v>
       </c>
     </row>
     <row r="10" ht="15" spans="1:3">
       <c r="A10" s="25"/>
       <c r="B10" s="7"/>
       <c r="C10" s="5" t="s">
-        <v>26</v>
+        <v>78</v>
       </c>
     </row>
     <row r="11" ht="15" spans="1:3">
       <c r="A11" s="25"/>
       <c r="B11" s="7"/>
       <c r="C11" s="5" t="s">
-        <v>27</v>
+        <v>79</v>
       </c>
     </row>
     <row r="12" ht="15" spans="1:3">
       <c r="A12" s="25"/>
       <c r="B12" s="7"/>
       <c r="C12" s="5" t="s">
-        <v>28</v>
+        <v>80</v>
       </c>
     </row>
     <row r="13" ht="15" spans="1:3">
       <c r="A13" s="25"/>
       <c r="B13" s="7"/>
       <c r="C13" s="5" t="s">
-        <v>29</v>
+        <v>81</v>
       </c>
     </row>
     <row r="14" ht="15" spans="1:3">
       <c r="A14" s="25"/>
       <c r="B14" s="7"/>
       <c r="C14" s="5" t="s">
-        <v>30</v>
+        <v>82</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -2600,94 +3231,94 @@
     <row r="16" ht="15" spans="1:3">
       <c r="A16" s="25"/>
       <c r="B16" s="7" t="s">
-        <v>31</v>
+        <v>83</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>32</v>
+        <v>84</v>
       </c>
     </row>
     <row r="17" ht="15" spans="1:3">
       <c r="A17" s="25"/>
       <c r="B17" s="7"/>
       <c r="C17" s="5" t="s">
-        <v>33</v>
+        <v>85</v>
       </c>
     </row>
     <row r="18" ht="15" spans="1:3">
       <c r="A18" s="25"/>
       <c r="B18" s="7"/>
       <c r="C18" s="5" t="s">
-        <v>34</v>
+        <v>86</v>
       </c>
     </row>
     <row r="19" ht="15" spans="1:3">
       <c r="A19" s="25"/>
       <c r="B19" s="7"/>
       <c r="C19" s="5" t="s">
-        <v>35</v>
+        <v>87</v>
       </c>
     </row>
     <row r="20" ht="15" spans="1:3">
       <c r="A20" s="25"/>
       <c r="B20" s="7"/>
       <c r="C20" s="5" t="s">
-        <v>36</v>
+        <v>88</v>
       </c>
     </row>
     <row r="21" ht="15" spans="1:3">
       <c r="A21" s="25"/>
       <c r="B21" s="7"/>
       <c r="C21" s="5" t="s">
-        <v>37</v>
+        <v>89</v>
       </c>
     </row>
     <row r="22" ht="15" spans="1:3">
       <c r="A22" s="25"/>
       <c r="B22" s="7"/>
       <c r="C22" s="5" t="s">
-        <v>38</v>
+        <v>90</v>
       </c>
     </row>
     <row r="23" ht="15" spans="1:3">
       <c r="A23" s="25"/>
       <c r="B23" s="7"/>
       <c r="C23" s="5" t="s">
-        <v>39</v>
+        <v>91</v>
       </c>
     </row>
     <row r="24" ht="15" spans="1:3">
       <c r="A24" s="25"/>
       <c r="B24" s="7"/>
       <c r="C24" s="5" t="s">
-        <v>40</v>
+        <v>92</v>
       </c>
     </row>
     <row r="25" ht="15" spans="1:3">
       <c r="A25" s="25"/>
       <c r="B25" s="7"/>
       <c r="C25" s="5" t="s">
-        <v>41</v>
+        <v>93</v>
       </c>
     </row>
     <row r="26" ht="15" spans="1:3">
       <c r="A26" s="25"/>
       <c r="B26" s="7"/>
       <c r="C26" s="5" t="s">
-        <v>42</v>
+        <v>94</v>
       </c>
     </row>
     <row r="27" ht="15" spans="1:3">
       <c r="A27" s="25"/>
       <c r="B27" s="7"/>
       <c r="C27" s="5" t="s">
-        <v>43</v>
+        <v>95</v>
       </c>
     </row>
     <row r="28" ht="15" spans="1:3">
       <c r="A28" s="25"/>
       <c r="B28" s="7"/>
       <c r="C28" s="5" t="s">
-        <v>44</v>
+        <v>96</v>
       </c>
     </row>
     <row r="29" spans="1:3">
@@ -2697,52 +3328,52 @@
     <row r="30" ht="15" spans="1:3">
       <c r="A30" s="25"/>
       <c r="B30" s="7" t="s">
-        <v>45</v>
+        <v>97</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>46</v>
+        <v>98</v>
       </c>
     </row>
     <row r="31" ht="15" spans="1:3">
       <c r="A31" s="25"/>
       <c r="B31" s="7"/>
       <c r="C31" s="5" t="s">
-        <v>47</v>
+        <v>99</v>
       </c>
     </row>
     <row r="32" ht="15" spans="1:3">
       <c r="A32" s="25"/>
       <c r="B32" s="7"/>
       <c r="C32" s="5" t="s">
-        <v>48</v>
+        <v>100</v>
       </c>
     </row>
     <row r="33" ht="15" spans="1:3">
       <c r="A33" s="25"/>
       <c r="B33" s="7"/>
       <c r="C33" s="5" t="s">
-        <v>49</v>
+        <v>101</v>
       </c>
     </row>
     <row r="34" ht="15" spans="1:3">
       <c r="A34" s="25"/>
       <c r="B34" s="7"/>
       <c r="C34" s="5" t="s">
-        <v>50</v>
+        <v>102</v>
       </c>
     </row>
     <row r="35" ht="15" spans="1:3">
       <c r="A35" s="25"/>
       <c r="B35" s="7"/>
       <c r="C35" s="5" t="s">
-        <v>51</v>
+        <v>103</v>
       </c>
     </row>
     <row r="36" ht="15" spans="1:3">
       <c r="A36" s="25"/>
       <c r="B36" s="7"/>
       <c r="C36" s="5" t="s">
-        <v>52</v>
+        <v>104</v>
       </c>
     </row>
     <row r="37" ht="15.75" spans="1:3">
@@ -2753,66 +3384,66 @@
     <row r="38" ht="15" spans="1:3">
       <c r="A38" s="25"/>
       <c r="B38" s="7" t="s">
-        <v>53</v>
+        <v>105</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>54</v>
+        <v>106</v>
       </c>
     </row>
     <row r="39" ht="15" spans="1:3">
       <c r="A39" s="25"/>
       <c r="B39" s="7"/>
       <c r="C39" s="5" t="s">
-        <v>55</v>
+        <v>107</v>
       </c>
     </row>
     <row r="40" ht="15" spans="1:3">
       <c r="A40" s="25"/>
       <c r="B40" s="7"/>
       <c r="C40" s="5" t="s">
-        <v>56</v>
+        <v>108</v>
       </c>
     </row>
     <row r="41" ht="15" spans="1:3">
       <c r="A41" s="25"/>
       <c r="B41" s="7"/>
       <c r="C41" s="5" t="s">
-        <v>57</v>
+        <v>109</v>
       </c>
     </row>
     <row r="42" ht="15" spans="1:3">
       <c r="A42" s="25"/>
       <c r="B42" s="7"/>
       <c r="C42" s="5" t="s">
-        <v>58</v>
+        <v>110</v>
       </c>
     </row>
     <row r="43" ht="15" spans="1:3">
       <c r="A43" s="25"/>
       <c r="B43" s="7"/>
       <c r="C43" s="5" t="s">
-        <v>59</v>
+        <v>111</v>
       </c>
     </row>
     <row r="44" ht="15" spans="1:3">
       <c r="A44" s="25"/>
       <c r="B44" s="7"/>
       <c r="C44" s="5" t="s">
-        <v>60</v>
+        <v>112</v>
       </c>
     </row>
     <row r="45" ht="15" spans="1:3">
       <c r="A45" s="25"/>
       <c r="B45" s="7"/>
       <c r="C45" s="5" t="s">
-        <v>61</v>
+        <v>113</v>
       </c>
     </row>
     <row r="46" ht="15" spans="1:3">
       <c r="A46" s="25"/>
       <c r="B46" s="7"/>
       <c r="C46" s="5" t="s">
-        <v>62</v>
+        <v>114</v>
       </c>
     </row>
     <row r="47" ht="15.75" spans="1:3">
@@ -2823,73 +3454,73 @@
     <row r="48" ht="15" spans="1:3">
       <c r="A48" s="25"/>
       <c r="B48" s="7" t="s">
-        <v>63</v>
+        <v>115</v>
       </c>
       <c r="C48" s="5" t="s">
-        <v>64</v>
+        <v>116</v>
       </c>
     </row>
     <row r="49" ht="15" spans="1:3">
       <c r="A49" s="25"/>
       <c r="B49" s="7"/>
       <c r="C49" s="5" t="s">
-        <v>47</v>
+        <v>99</v>
       </c>
     </row>
     <row r="50" ht="15" spans="1:3">
       <c r="A50" s="25"/>
       <c r="B50" s="7"/>
       <c r="C50" s="5" t="s">
-        <v>65</v>
+        <v>117</v>
       </c>
     </row>
     <row r="51" ht="15" spans="1:3">
       <c r="A51" s="25"/>
       <c r="B51" s="7"/>
       <c r="C51" s="5" t="s">
-        <v>66</v>
+        <v>118</v>
       </c>
     </row>
     <row r="52" ht="15" spans="1:3">
       <c r="A52" s="25"/>
       <c r="B52" s="7"/>
       <c r="C52" s="5" t="s">
-        <v>67</v>
+        <v>119</v>
       </c>
     </row>
     <row r="53" ht="15" spans="1:3">
       <c r="A53" s="25"/>
       <c r="B53" s="7"/>
       <c r="C53" s="5" t="s">
-        <v>51</v>
+        <v>103</v>
       </c>
     </row>
     <row r="54" ht="15" spans="1:3">
       <c r="A54" s="25"/>
       <c r="B54" s="7"/>
       <c r="C54" s="5" t="s">
-        <v>52</v>
+        <v>104</v>
       </c>
     </row>
     <row r="55" ht="15" spans="1:3">
       <c r="A55" s="25"/>
       <c r="B55" s="7"/>
       <c r="C55" s="5" t="s">
-        <v>68</v>
+        <v>120</v>
       </c>
     </row>
     <row r="56" ht="15" spans="1:3">
       <c r="A56" s="25"/>
       <c r="B56" s="7"/>
       <c r="C56" s="5" t="s">
-        <v>69</v>
+        <v>121</v>
       </c>
     </row>
     <row r="57" ht="15" spans="1:3">
       <c r="A57" s="25"/>
       <c r="B57" s="7"/>
       <c r="C57" s="5" t="s">
-        <v>30</v>
+        <v>82</v>
       </c>
     </row>
     <row r="58" ht="15" spans="1:3">
@@ -2899,59 +3530,59 @@
     <row r="59" ht="15" spans="1:3">
       <c r="A59" s="25"/>
       <c r="B59" s="7" t="s">
-        <v>70</v>
+        <v>122</v>
       </c>
       <c r="C59" s="5" t="s">
-        <v>71</v>
+        <v>123</v>
       </c>
     </row>
     <row r="60" ht="15" spans="1:3">
       <c r="A60" s="25"/>
       <c r="B60" s="7"/>
       <c r="C60" s="5" t="s">
-        <v>72</v>
+        <v>124</v>
       </c>
     </row>
     <row r="61" ht="15" spans="1:3">
       <c r="A61" s="25"/>
       <c r="B61" s="7"/>
       <c r="C61" s="5" t="s">
-        <v>73</v>
+        <v>125</v>
       </c>
     </row>
     <row r="62" ht="15" spans="1:3">
       <c r="A62" s="25"/>
       <c r="B62" s="7"/>
       <c r="C62" s="5" t="s">
-        <v>66</v>
+        <v>118</v>
       </c>
     </row>
     <row r="63" ht="15" spans="1:3">
       <c r="A63" s="25"/>
       <c r="B63" s="7"/>
       <c r="C63" s="5" t="s">
-        <v>74</v>
+        <v>126</v>
       </c>
     </row>
     <row r="64" ht="15" spans="1:3">
       <c r="A64" s="25"/>
       <c r="B64" s="7"/>
       <c r="C64" s="5" t="s">
-        <v>75</v>
+        <v>127</v>
       </c>
     </row>
     <row r="65" ht="15" spans="1:3">
       <c r="A65" s="25"/>
       <c r="B65" s="7"/>
       <c r="C65" s="5" t="s">
-        <v>76</v>
+        <v>128</v>
       </c>
     </row>
     <row r="66" ht="15" spans="1:3">
       <c r="A66" s="25"/>
       <c r="B66" s="7"/>
       <c r="C66" s="5" t="s">
-        <v>77</v>
+        <v>129</v>
       </c>
     </row>
     <row r="67" ht="15" spans="1:3">
@@ -2961,31 +3592,31 @@
     <row r="68" ht="15" spans="1:3">
       <c r="A68" s="25"/>
       <c r="B68" s="9" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="C68" s="10" t="s">
-        <v>79</v>
+        <v>130</v>
       </c>
     </row>
     <row r="69" ht="15" spans="1:3">
       <c r="A69" s="25"/>
       <c r="B69" s="9"/>
       <c r="C69" s="5" t="s">
-        <v>80</v>
+        <v>131</v>
       </c>
     </row>
     <row r="70" ht="15" spans="1:3">
       <c r="A70" s="25"/>
       <c r="B70" s="9"/>
       <c r="C70" s="5" t="s">
-        <v>81</v>
+        <v>132</v>
       </c>
     </row>
     <row r="71" spans="1:3">
       <c r="A71" s="25"/>
       <c r="B71" s="9"/>
       <c r="C71" s="26" t="s">
-        <v>82</v>
+        <v>133</v>
       </c>
     </row>
     <row r="72" hidden="1" spans="1:3">
@@ -2997,7 +3628,7 @@
       <c r="A73" s="25"/>
       <c r="B73" s="9"/>
       <c r="C73" s="26" t="s">
-        <v>83</v>
+        <v>134</v>
       </c>
     </row>
     <row r="74" ht="9" customHeight="1" spans="1:3">
@@ -3007,7 +3638,7 @@
     </row>
     <row r="77" ht="18.75" spans="1:2">
       <c r="A77" s="19" t="s">
-        <v>84</v>
+        <v>135</v>
       </c>
       <c r="B77" s="20">
         <v>1</v>
@@ -3015,7 +3646,7 @@
     </row>
     <row r="78" ht="18.75" spans="1:2">
       <c r="A78" s="19" t="s">
-        <v>85</v>
+        <v>136</v>
       </c>
       <c r="B78" s="20">
         <v>8</v>
@@ -3039,7 +3670,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
   <dimension ref="A1:C68"/>
@@ -3071,14 +3702,14 @@
     </row>
     <row r="2" ht="24.75" spans="1:3">
       <c r="A2" s="2" t="s">
-        <v>86</v>
+        <v>137</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
     </row>
     <row r="3" ht="15.75" spans="1:3">
       <c r="A3" s="3" t="s">
-        <v>87</v>
+        <v>138</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>20</v>
@@ -3095,45 +3726,45 @@
     <row r="5" ht="15" spans="1:3">
       <c r="A5" s="6"/>
       <c r="B5" s="7" t="s">
-        <v>88</v>
+        <v>139</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>22</v>
+        <v>74</v>
       </c>
     </row>
     <row r="6" ht="15" spans="1:3">
       <c r="A6" s="6"/>
       <c r="B6" s="7"/>
       <c r="C6" s="5" t="s">
-        <v>89</v>
+        <v>140</v>
       </c>
     </row>
     <row r="7" ht="15" spans="1:3">
       <c r="A7" s="6"/>
       <c r="B7" s="7"/>
       <c r="C7" s="5" t="s">
-        <v>90</v>
+        <v>141</v>
       </c>
     </row>
     <row r="8" ht="15" spans="1:3">
       <c r="A8" s="6"/>
       <c r="B8" s="7"/>
       <c r="C8" s="5" t="s">
-        <v>91</v>
+        <v>142</v>
       </c>
     </row>
     <row r="9" ht="15" spans="1:3">
       <c r="A9" s="6"/>
       <c r="B9" s="7"/>
       <c r="C9" s="5" t="s">
-        <v>92</v>
+        <v>143</v>
       </c>
     </row>
     <row r="10" ht="15" spans="1:3">
       <c r="A10" s="6"/>
       <c r="B10" s="7"/>
       <c r="C10" s="5" t="s">
-        <v>93</v>
+        <v>144</v>
       </c>
     </row>
     <row r="11" ht="15.75" spans="1:3">
@@ -3144,52 +3775,52 @@
     <row r="12" ht="15" spans="1:3">
       <c r="A12" s="6"/>
       <c r="B12" s="7" t="s">
-        <v>94</v>
+        <v>145</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>22</v>
+        <v>74</v>
       </c>
     </row>
     <row r="13" ht="15" spans="1:3">
       <c r="A13" s="6"/>
       <c r="B13" s="7"/>
       <c r="C13" s="5" t="s">
-        <v>95</v>
+        <v>146</v>
       </c>
     </row>
     <row r="14" ht="15" spans="1:3">
       <c r="A14" s="6"/>
       <c r="B14" s="7"/>
       <c r="C14" s="5" t="s">
-        <v>96</v>
+        <v>147</v>
       </c>
     </row>
     <row r="15" ht="15" spans="1:3">
       <c r="A15" s="6"/>
       <c r="B15" s="7"/>
       <c r="C15" s="5" t="s">
-        <v>97</v>
+        <v>148</v>
       </c>
     </row>
     <row r="16" ht="15" spans="1:3">
       <c r="A16" s="6"/>
       <c r="B16" s="7"/>
       <c r="C16" s="5" t="s">
-        <v>98</v>
+        <v>149</v>
       </c>
     </row>
     <row r="17" ht="15" spans="1:3">
       <c r="A17" s="6"/>
       <c r="B17" s="7"/>
       <c r="C17" s="5" t="s">
-        <v>99</v>
+        <v>150</v>
       </c>
     </row>
     <row r="18" ht="15" spans="1:3">
       <c r="A18" s="6"/>
       <c r="B18" s="7"/>
       <c r="C18" s="5" t="s">
-        <v>100</v>
+        <v>151</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -3199,38 +3830,38 @@
     <row r="20" ht="15" spans="1:3">
       <c r="A20" s="6"/>
       <c r="B20" s="7" t="s">
-        <v>101</v>
+        <v>152</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>22</v>
+        <v>74</v>
       </c>
     </row>
     <row r="21" ht="15" spans="1:3">
       <c r="A21" s="6"/>
       <c r="B21" s="7"/>
       <c r="C21" s="5" t="s">
-        <v>102</v>
+        <v>153</v>
       </c>
     </row>
     <row r="22" ht="15" spans="1:3">
       <c r="A22" s="6"/>
       <c r="B22" s="7"/>
       <c r="C22" s="5" t="s">
-        <v>103</v>
+        <v>154</v>
       </c>
     </row>
     <row r="23" ht="15" spans="1:3">
       <c r="A23" s="6"/>
       <c r="B23" s="7"/>
       <c r="C23" s="5" t="s">
-        <v>104</v>
+        <v>155</v>
       </c>
     </row>
     <row r="24" ht="15" spans="1:3">
       <c r="A24" s="6"/>
       <c r="B24" s="7"/>
       <c r="C24" s="5" t="s">
-        <v>105</v>
+        <v>156</v>
       </c>
     </row>
     <row r="25" ht="15" spans="1:3">
@@ -3241,52 +3872,52 @@
     <row r="26" ht="15" spans="1:3">
       <c r="A26" s="6"/>
       <c r="B26" s="7" t="s">
-        <v>106</v>
+        <v>157</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>22</v>
+        <v>74</v>
       </c>
     </row>
     <row r="27" ht="15" spans="1:3">
       <c r="A27" s="6"/>
       <c r="B27" s="7"/>
       <c r="C27" s="5" t="s">
-        <v>107</v>
+        <v>158</v>
       </c>
     </row>
     <row r="28" ht="15" spans="1:3">
       <c r="A28" s="6"/>
       <c r="B28" s="7"/>
       <c r="C28" s="5" t="s">
-        <v>108</v>
+        <v>159</v>
       </c>
     </row>
     <row r="29" ht="15" spans="1:3">
       <c r="A29" s="6"/>
       <c r="B29" s="7"/>
       <c r="C29" s="5" t="s">
-        <v>109</v>
+        <v>160</v>
       </c>
     </row>
     <row r="30" ht="15" spans="1:3">
       <c r="A30" s="6"/>
       <c r="B30" s="7"/>
       <c r="C30" s="5" t="s">
-        <v>110</v>
+        <v>161</v>
       </c>
     </row>
     <row r="31" ht="15" spans="1:3">
       <c r="A31" s="6"/>
       <c r="B31" s="7"/>
       <c r="C31" s="5" t="s">
-        <v>111</v>
+        <v>162</v>
       </c>
     </row>
     <row r="32" ht="15" spans="1:3">
       <c r="A32" s="6"/>
       <c r="B32" s="7"/>
       <c r="C32" s="5" t="s">
-        <v>100</v>
+        <v>151</v>
       </c>
     </row>
     <row r="33" ht="15" spans="1:3">
@@ -3296,48 +3927,48 @@
     </row>
     <row r="34" ht="15" spans="1:3">
       <c r="A34" s="6" t="s">
-        <v>112</v>
+        <v>163</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>113</v>
+        <v>164</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>22</v>
+        <v>74</v>
       </c>
     </row>
     <row r="35" ht="15" spans="1:3">
       <c r="A35" s="6"/>
       <c r="B35" s="7"/>
       <c r="C35" s="5" t="s">
-        <v>114</v>
+        <v>165</v>
       </c>
     </row>
     <row r="36" ht="15" spans="1:3">
       <c r="A36" s="6"/>
       <c r="B36" s="7"/>
       <c r="C36" s="5" t="s">
-        <v>115</v>
+        <v>166</v>
       </c>
     </row>
     <row r="37" ht="15" spans="1:3">
       <c r="A37" s="6"/>
       <c r="B37" s="7"/>
       <c r="C37" s="5" t="s">
-        <v>116</v>
+        <v>167</v>
       </c>
     </row>
     <row r="38" ht="15" spans="1:3">
       <c r="A38" s="6"/>
       <c r="B38" s="7"/>
       <c r="C38" s="5" t="s">
-        <v>117</v>
+        <v>168</v>
       </c>
     </row>
     <row r="39" ht="15" spans="1:3">
       <c r="A39" s="6"/>
       <c r="B39" s="7"/>
       <c r="C39" s="5" t="s">
-        <v>93</v>
+        <v>144</v>
       </c>
     </row>
     <row r="40" spans="1:3">
@@ -3347,38 +3978,38 @@
     <row r="41" ht="15" spans="1:3">
       <c r="A41" s="6"/>
       <c r="B41" s="7" t="s">
-        <v>118</v>
+        <v>169</v>
       </c>
       <c r="C41" s="23" t="s">
-        <v>22</v>
+        <v>74</v>
       </c>
     </row>
     <row r="42" ht="15" spans="1:3">
       <c r="A42" s="6"/>
       <c r="B42" s="7"/>
       <c r="C42" s="5" t="s">
-        <v>119</v>
+        <v>170</v>
       </c>
     </row>
     <row r="43" ht="15" spans="1:3">
       <c r="A43" s="6"/>
       <c r="B43" s="7"/>
       <c r="C43" s="5" t="s">
-        <v>120</v>
+        <v>171</v>
       </c>
     </row>
     <row r="44" ht="15" spans="1:3">
       <c r="A44" s="6"/>
       <c r="B44" s="7"/>
       <c r="C44" s="5" t="s">
-        <v>121</v>
+        <v>172</v>
       </c>
     </row>
     <row r="45" ht="15" spans="1:3">
       <c r="A45" s="6"/>
       <c r="B45" s="7"/>
       <c r="C45" s="5" t="s">
-        <v>105</v>
+        <v>156</v>
       </c>
     </row>
     <row r="46" ht="18" spans="1:3">
@@ -3389,45 +4020,45 @@
     <row r="47" ht="15" spans="1:3">
       <c r="A47" s="6"/>
       <c r="B47" s="7" t="s">
-        <v>122</v>
+        <v>173</v>
       </c>
       <c r="C47" s="23" t="s">
-        <v>22</v>
+        <v>74</v>
       </c>
     </row>
     <row r="48" ht="15" spans="1:3">
       <c r="A48" s="6"/>
       <c r="B48" s="7"/>
       <c r="C48" s="5" t="s">
-        <v>123</v>
+        <v>174</v>
       </c>
     </row>
     <row r="49" ht="15" spans="1:3">
       <c r="A49" s="6"/>
       <c r="B49" s="7"/>
       <c r="C49" s="5" t="s">
-        <v>124</v>
+        <v>175</v>
       </c>
     </row>
     <row r="50" ht="15" spans="1:3">
       <c r="A50" s="6"/>
       <c r="B50" s="7"/>
       <c r="C50" s="5" t="s">
-        <v>125</v>
+        <v>176</v>
       </c>
     </row>
     <row r="51" ht="15" spans="1:3">
       <c r="A51" s="6"/>
       <c r="B51" s="7"/>
       <c r="C51" s="5" t="s">
-        <v>126</v>
+        <v>177</v>
       </c>
     </row>
     <row r="52" ht="15" spans="1:3">
       <c r="A52" s="6"/>
       <c r="B52" s="7"/>
       <c r="C52" s="5" t="s">
-        <v>93</v>
+        <v>144</v>
       </c>
     </row>
     <row r="53" ht="15" spans="1:3">
@@ -3438,45 +4069,45 @@
     <row r="54" ht="15" spans="1:3">
       <c r="A54" s="6"/>
       <c r="B54" s="7" t="s">
-        <v>127</v>
+        <v>178</v>
       </c>
       <c r="C54" s="5" t="s">
-        <v>22</v>
+        <v>74</v>
       </c>
     </row>
     <row r="55" ht="15" spans="1:3">
       <c r="A55" s="6"/>
       <c r="B55" s="7"/>
       <c r="C55" s="5" t="s">
-        <v>128</v>
+        <v>179</v>
       </c>
     </row>
     <row r="56" ht="15" spans="1:3">
       <c r="A56" s="6"/>
       <c r="B56" s="7"/>
       <c r="C56" s="5" t="s">
-        <v>129</v>
+        <v>180</v>
       </c>
     </row>
     <row r="57" ht="15" spans="1:3">
       <c r="A57" s="6"/>
       <c r="B57" s="7"/>
       <c r="C57" s="5" t="s">
-        <v>130</v>
+        <v>181</v>
       </c>
     </row>
     <row r="58" ht="15" spans="1:3">
       <c r="A58" s="6"/>
       <c r="B58" s="7"/>
       <c r="C58" s="5" t="s">
-        <v>131</v>
+        <v>182</v>
       </c>
     </row>
     <row r="59" ht="15" spans="1:3">
       <c r="A59" s="6"/>
       <c r="B59" s="7"/>
       <c r="C59" s="5" t="s">
-        <v>93</v>
+        <v>144</v>
       </c>
     </row>
     <row r="60" ht="15" spans="1:3">
@@ -3487,24 +4118,24 @@
     <row r="61" ht="15" spans="1:3">
       <c r="A61" s="6"/>
       <c r="B61" s="9" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="C61" s="10" t="s">
-        <v>132</v>
+        <v>183</v>
       </c>
     </row>
     <row r="62" ht="15" spans="1:3">
       <c r="A62" s="6"/>
       <c r="B62" s="9"/>
       <c r="C62" s="11" t="s">
-        <v>133</v>
+        <v>184</v>
       </c>
     </row>
     <row r="63" spans="1:3">
       <c r="A63" s="6"/>
       <c r="B63" s="9"/>
       <c r="C63" t="s">
-        <v>134</v>
+        <v>185</v>
       </c>
     </row>
     <row r="64" ht="9" customHeight="1" spans="1:3">
@@ -3514,7 +4145,7 @@
     </row>
     <row r="67" ht="18.75" spans="1:2">
       <c r="A67" s="19" t="s">
-        <v>135</v>
+        <v>186</v>
       </c>
       <c r="B67" s="20">
         <v>1</v>
@@ -3522,7 +4153,7 @@
     </row>
     <row r="68" ht="18.75" spans="1:2">
       <c r="A68" s="19" t="s">
-        <v>136</v>
+        <v>187</v>
       </c>
       <c r="B68" s="20">
         <v>8</v>
@@ -3548,13 +4179,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
   <dimension ref="A1:C29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
       <selection pane="bottomLeft" activeCell="D7" sqref="D7"/>
     </sheetView>
@@ -3580,14 +4211,14 @@
     </row>
     <row r="2" ht="24.75" spans="1:3">
       <c r="A2" s="2" t="s">
-        <v>137</v>
+        <v>188</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
     </row>
     <row r="3" ht="15.75" spans="1:3">
       <c r="A3" s="3" t="s">
-        <v>138</v>
+        <v>189</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>20</v>
@@ -3604,10 +4235,10 @@
     <row r="5" ht="15.75" spans="1:3">
       <c r="A5" s="3"/>
       <c r="B5" s="7" t="s">
-        <v>139</v>
+        <v>190</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>140</v>
+        <v>191</v>
       </c>
     </row>
     <row r="6" ht="15.75" spans="1:3">
@@ -3618,24 +4249,24 @@
     <row r="7" ht="15" spans="1:3">
       <c r="A7" s="3"/>
       <c r="B7" s="7" t="s">
-        <v>141</v>
+        <v>192</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>142</v>
+        <v>193</v>
       </c>
     </row>
     <row r="8" ht="15" spans="1:3">
       <c r="A8" s="3"/>
       <c r="B8" s="7"/>
       <c r="C8" s="5" t="s">
-        <v>143</v>
+        <v>194</v>
       </c>
     </row>
     <row r="9" ht="15" spans="1:3">
       <c r="A9" s="3"/>
       <c r="B9" s="7"/>
       <c r="C9" s="5" t="s">
-        <v>144</v>
+        <v>195</v>
       </c>
     </row>
     <row r="10" ht="18.75" spans="1:3">
@@ -3646,24 +4277,24 @@
     <row r="11" ht="15" spans="1:3">
       <c r="A11" s="3"/>
       <c r="B11" s="7" t="s">
-        <v>145</v>
+        <v>196</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>22</v>
+        <v>74</v>
       </c>
     </row>
     <row r="12" ht="15" spans="1:3">
       <c r="A12" s="3"/>
       <c r="B12" s="7"/>
       <c r="C12" s="5" t="s">
-        <v>146</v>
+        <v>197</v>
       </c>
     </row>
     <row r="13" ht="15" spans="1:3">
       <c r="A13" s="3"/>
       <c r="B13" s="7"/>
       <c r="C13" s="5" t="s">
-        <v>147</v>
+        <v>198</v>
       </c>
     </row>
     <row r="14" ht="15.75" spans="1:3">
@@ -3674,24 +4305,24 @@
     <row r="15" ht="15" spans="1:3">
       <c r="A15" s="3"/>
       <c r="B15" s="7" t="s">
-        <v>148</v>
+        <v>199</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>22</v>
+        <v>74</v>
       </c>
     </row>
     <row r="16" ht="15" spans="1:3">
       <c r="A16" s="3"/>
       <c r="B16" s="7"/>
       <c r="C16" s="5" t="s">
-        <v>149</v>
+        <v>200</v>
       </c>
     </row>
     <row r="17" ht="15" spans="1:3">
       <c r="A17" s="3"/>
       <c r="B17" s="7"/>
       <c r="C17" s="5" t="s">
-        <v>150</v>
+        <v>201</v>
       </c>
     </row>
     <row r="18" ht="15" spans="1:3">
@@ -3702,40 +4333,40 @@
     <row r="19" ht="15" spans="1:3">
       <c r="A19" s="3"/>
       <c r="B19" s="7" t="s">
-        <v>151</v>
+        <v>202</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>152</v>
+        <v>203</v>
       </c>
     </row>
     <row r="20" ht="15" spans="1:3">
       <c r="A20" s="3"/>
       <c r="B20" s="7"/>
       <c r="C20" s="5" t="s">
-        <v>153</v>
+        <v>204</v>
       </c>
     </row>
     <row r="21" ht="15" spans="1:3">
       <c r="A21" s="3"/>
       <c r="B21" s="7"/>
       <c r="C21" s="5" t="s">
-        <v>154</v>
+        <v>205</v>
       </c>
     </row>
     <row r="22" ht="15" spans="1:3">
       <c r="A22" s="3"/>
       <c r="B22" s="9" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="C22" s="10" t="s">
-        <v>155</v>
+        <v>206</v>
       </c>
     </row>
     <row r="23" ht="20" customHeight="1" spans="1:3">
       <c r="A23" s="3"/>
       <c r="B23" s="9"/>
       <c r="C23" s="22" t="s">
-        <v>156</v>
+        <v>207</v>
       </c>
     </row>
     <row r="24" spans="1:3">
@@ -3750,7 +4381,7 @@
     </row>
     <row r="28" ht="18.75" spans="1:2">
       <c r="A28" s="19" t="s">
-        <v>157</v>
+        <v>208</v>
       </c>
       <c r="B28" s="20">
         <v>1</v>
@@ -3758,7 +4389,7 @@
     </row>
     <row r="29" ht="18.75" spans="1:2">
       <c r="A29" s="19" t="s">
-        <v>158</v>
+        <v>209</v>
       </c>
       <c r="B29" s="20">
         <v>8</v>
@@ -3780,13 +4411,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
   <dimension ref="A1:C131"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A126" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A91" activePane="bottomLeft" state="frozen"/>
       <selection/>
       <selection pane="bottomLeft" activeCell="A98" sqref="A98:C98"/>
     </sheetView>
@@ -3811,14 +4442,14 @@
     </row>
     <row r="2" ht="24.75" spans="1:3">
       <c r="A2" s="2" t="s">
-        <v>159</v>
+        <v>210</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
     </row>
     <row r="3" ht="15.75" spans="1:3">
       <c r="A3" s="6" t="s">
-        <v>160</v>
+        <v>211</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>20</v>
@@ -3835,7 +4466,7 @@
     <row r="5" ht="15" spans="1:3">
       <c r="A5" s="6"/>
       <c r="B5" s="7" t="s">
-        <v>161</v>
+        <v>212</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>20</v>
@@ -3845,42 +4476,42 @@
       <c r="A6" s="6"/>
       <c r="B6" s="7"/>
       <c r="C6" s="5" t="s">
-        <v>162</v>
+        <v>213</v>
       </c>
     </row>
     <row r="7" ht="15" spans="1:3">
       <c r="A7" s="6"/>
       <c r="B7" s="7"/>
       <c r="C7" s="5" t="s">
-        <v>163</v>
+        <v>214</v>
       </c>
     </row>
     <row r="8" ht="15" spans="1:3">
       <c r="A8" s="6"/>
       <c r="B8" s="7"/>
       <c r="C8" s="5" t="s">
-        <v>164</v>
+        <v>215</v>
       </c>
     </row>
     <row r="9" ht="15" spans="1:3">
       <c r="A9" s="6"/>
       <c r="B9" s="7"/>
       <c r="C9" s="5" t="s">
-        <v>165</v>
+        <v>216</v>
       </c>
     </row>
     <row r="10" ht="15" spans="1:3">
       <c r="A10" s="6"/>
       <c r="B10" s="7"/>
       <c r="C10" s="5" t="s">
-        <v>26</v>
+        <v>78</v>
       </c>
     </row>
     <row r="11" ht="15" spans="1:3">
       <c r="A11" s="6"/>
       <c r="B11" s="7"/>
       <c r="C11" s="5" t="s">
-        <v>100</v>
+        <v>151</v>
       </c>
     </row>
     <row r="12" ht="15.75" spans="1:3">
@@ -3891,66 +4522,66 @@
     <row r="13" ht="18.75" spans="1:3">
       <c r="A13" s="6"/>
       <c r="B13" s="7" t="s">
-        <v>166</v>
+        <v>217</v>
       </c>
       <c r="C13" s="15" t="s">
-        <v>22</v>
+        <v>74</v>
       </c>
     </row>
     <row r="14" ht="15" spans="1:3">
       <c r="A14" s="6"/>
       <c r="B14" s="7"/>
       <c r="C14" s="5" t="s">
-        <v>167</v>
+        <v>218</v>
       </c>
     </row>
     <row r="15" ht="18.75" spans="1:3">
       <c r="A15" s="6"/>
       <c r="B15" s="7"/>
       <c r="C15" s="15" t="s">
-        <v>34</v>
+        <v>86</v>
       </c>
     </row>
     <row r="16" ht="18.75" spans="1:3">
       <c r="A16" s="6"/>
       <c r="B16" s="7"/>
       <c r="C16" s="15" t="s">
-        <v>168</v>
+        <v>219</v>
       </c>
     </row>
     <row r="17" ht="18.75" spans="1:3">
       <c r="A17" s="6"/>
       <c r="B17" s="7"/>
       <c r="C17" s="15" t="s">
-        <v>169</v>
+        <v>220</v>
       </c>
     </row>
     <row r="18" ht="18.75" spans="1:3">
       <c r="A18" s="6"/>
       <c r="B18" s="7"/>
       <c r="C18" s="15" t="s">
-        <v>170</v>
+        <v>221</v>
       </c>
     </row>
     <row r="19" ht="18.75" spans="1:3">
       <c r="A19" s="6"/>
       <c r="B19" s="7"/>
       <c r="C19" s="15" t="s">
-        <v>171</v>
+        <v>222</v>
       </c>
     </row>
     <row r="20" ht="18.75" spans="1:3">
       <c r="A20" s="6"/>
       <c r="B20" s="7"/>
       <c r="C20" s="15" t="s">
-        <v>172</v>
+        <v>223</v>
       </c>
     </row>
     <row r="21" ht="18.75" spans="1:3">
       <c r="A21" s="6"/>
       <c r="B21" s="7"/>
       <c r="C21" s="15" t="s">
-        <v>62</v>
+        <v>114</v>
       </c>
     </row>
     <row r="22" spans="1:3">
@@ -3960,66 +4591,66 @@
     <row r="23" ht="18.75" spans="1:3">
       <c r="A23" s="6"/>
       <c r="B23" s="7" t="s">
-        <v>173</v>
+        <v>224</v>
       </c>
       <c r="C23" s="15" t="s">
-        <v>22</v>
+        <v>74</v>
       </c>
     </row>
     <row r="24" ht="18.75" spans="1:3">
       <c r="A24" s="6"/>
       <c r="B24" s="7"/>
       <c r="C24" s="15" t="s">
-        <v>33</v>
+        <v>85</v>
       </c>
     </row>
     <row r="25" ht="18.75" spans="1:3">
       <c r="A25" s="6"/>
       <c r="B25" s="7"/>
       <c r="C25" s="15" t="s">
-        <v>174</v>
+        <v>225</v>
       </c>
     </row>
     <row r="26" ht="18.75" spans="1:3">
       <c r="A26" s="6"/>
       <c r="B26" s="7"/>
       <c r="C26" s="15" t="s">
-        <v>175</v>
+        <v>226</v>
       </c>
     </row>
     <row r="27" ht="18.75" spans="1:3">
       <c r="A27" s="6"/>
       <c r="B27" s="7"/>
       <c r="C27" s="15" t="s">
-        <v>176</v>
+        <v>227</v>
       </c>
     </row>
     <row r="28" ht="18.75" spans="1:3">
       <c r="A28" s="6"/>
       <c r="B28" s="7"/>
       <c r="C28" s="15" t="s">
-        <v>177</v>
+        <v>228</v>
       </c>
     </row>
     <row r="29" ht="18.75" spans="1:3">
       <c r="A29" s="6"/>
       <c r="B29" s="7"/>
       <c r="C29" s="15" t="s">
-        <v>178</v>
+        <v>229</v>
       </c>
     </row>
     <row r="30" ht="18.75" spans="1:3">
       <c r="A30" s="6"/>
       <c r="B30" s="7"/>
       <c r="C30" s="15" t="s">
-        <v>179</v>
+        <v>230</v>
       </c>
     </row>
     <row r="31" ht="18.75" spans="1:3">
       <c r="A31" s="6"/>
       <c r="B31" s="7"/>
       <c r="C31" s="15" t="s">
-        <v>62</v>
+        <v>114</v>
       </c>
     </row>
     <row r="32" spans="1:3">
@@ -4030,87 +4661,87 @@
     <row r="33" ht="18.75" spans="1:3">
       <c r="A33" s="6"/>
       <c r="B33" s="7" t="s">
-        <v>180</v>
+        <v>231</v>
       </c>
       <c r="C33" s="15" t="s">
-        <v>22</v>
+        <v>74</v>
       </c>
     </row>
     <row r="34" ht="18.75" spans="1:3">
       <c r="A34" s="6"/>
       <c r="B34" s="7"/>
       <c r="C34" s="15" t="s">
-        <v>181</v>
+        <v>232</v>
       </c>
     </row>
     <row r="35" ht="18.75" spans="1:3">
       <c r="A35" s="6"/>
       <c r="B35" s="7"/>
       <c r="C35" s="15" t="s">
-        <v>182</v>
+        <v>233</v>
       </c>
     </row>
     <row r="36" ht="18.75" spans="1:3">
       <c r="A36" s="6"/>
       <c r="B36" s="7"/>
       <c r="C36" s="15" t="s">
-        <v>183</v>
+        <v>234</v>
       </c>
     </row>
     <row r="37" ht="18.75" spans="1:3">
       <c r="A37" s="6"/>
       <c r="B37" s="7"/>
       <c r="C37" s="15" t="s">
-        <v>184</v>
+        <v>235</v>
       </c>
     </row>
     <row r="38" ht="18.75" spans="1:3">
       <c r="A38" s="6"/>
       <c r="B38" s="7"/>
       <c r="C38" s="15" t="s">
-        <v>185</v>
+        <v>236</v>
       </c>
     </row>
     <row r="39" ht="18.75" spans="1:3">
       <c r="A39" s="6"/>
       <c r="B39" s="7"/>
       <c r="C39" s="15" t="s">
-        <v>186</v>
+        <v>237</v>
       </c>
     </row>
     <row r="40" ht="18.75" spans="1:3">
       <c r="A40" s="6"/>
       <c r="B40" s="7"/>
       <c r="C40" s="15" t="s">
-        <v>187</v>
+        <v>238</v>
       </c>
     </row>
     <row r="41" ht="18.75" spans="1:3">
       <c r="A41" s="6"/>
       <c r="B41" s="7"/>
       <c r="C41" s="15" t="s">
-        <v>188</v>
+        <v>239</v>
       </c>
     </row>
     <row r="42" ht="18.75" spans="1:3">
       <c r="A42" s="6"/>
       <c r="B42" s="7"/>
       <c r="C42" s="15" t="s">
-        <v>189</v>
+        <v>240</v>
       </c>
     </row>
     <row r="43" ht="18.75" spans="1:3">
       <c r="A43" s="6"/>
       <c r="B43" s="7"/>
       <c r="C43" s="15" t="s">
-        <v>190</v>
+        <v>241</v>
       </c>
     </row>
     <row r="44" ht="18.75" spans="1:3">
       <c r="A44" s="6"/>
       <c r="B44" s="7"/>
       <c r="C44" s="15" t="s">
-        <v>191</v>
+        <v>242</v>
       </c>
     </row>
     <row r="45" spans="1:3">
@@ -4120,129 +4751,129 @@
     <row r="46" ht="18.75" spans="1:3">
       <c r="A46" s="6"/>
       <c r="B46" s="7" t="s">
-        <v>192</v>
+        <v>243</v>
       </c>
       <c r="C46" s="15" t="s">
-        <v>22</v>
+        <v>74</v>
       </c>
     </row>
     <row r="47" ht="18.75" spans="1:3">
       <c r="A47" s="6"/>
       <c r="B47" s="7"/>
       <c r="C47" s="15" t="s">
-        <v>193</v>
+        <v>244</v>
       </c>
     </row>
     <row r="48" ht="18.75" spans="1:3">
       <c r="A48" s="6"/>
       <c r="B48" s="7"/>
       <c r="C48" s="15" t="s">
-        <v>194</v>
+        <v>245</v>
       </c>
     </row>
     <row r="49" ht="18.75" spans="1:3">
       <c r="A49" s="6"/>
       <c r="B49" s="7"/>
       <c r="C49" s="15" t="s">
-        <v>195</v>
+        <v>246</v>
       </c>
     </row>
     <row r="50" ht="18.75" spans="1:3">
       <c r="A50" s="6"/>
       <c r="B50" s="7"/>
       <c r="C50" s="15" t="s">
-        <v>196</v>
+        <v>247</v>
       </c>
     </row>
     <row r="51" ht="18.75" spans="1:3">
       <c r="A51" s="6"/>
       <c r="B51" s="7"/>
       <c r="C51" s="15" t="s">
-        <v>197</v>
+        <v>248</v>
       </c>
     </row>
     <row r="52" ht="18.75" spans="1:3">
       <c r="A52" s="6"/>
       <c r="B52" s="7"/>
       <c r="C52" s="15" t="s">
-        <v>198</v>
+        <v>249</v>
       </c>
     </row>
     <row r="53" ht="18.75" spans="1:3">
       <c r="A53" s="6"/>
       <c r="B53" s="7"/>
       <c r="C53" s="15" t="s">
-        <v>199</v>
+        <v>250</v>
       </c>
     </row>
     <row r="54" ht="18.75" spans="1:3">
       <c r="A54" s="6"/>
       <c r="B54" s="7"/>
       <c r="C54" s="15" t="s">
-        <v>200</v>
+        <v>251</v>
       </c>
     </row>
     <row r="55" ht="18.75" spans="1:3">
       <c r="A55" s="6"/>
       <c r="B55" s="7"/>
       <c r="C55" s="15" t="s">
-        <v>201</v>
+        <v>252</v>
       </c>
     </row>
     <row r="56" ht="18.75" spans="1:3">
       <c r="A56" s="6"/>
       <c r="B56" s="7"/>
       <c r="C56" s="15" t="s">
-        <v>202</v>
+        <v>253</v>
       </c>
     </row>
     <row r="57" ht="18.75" spans="1:3">
       <c r="A57" s="6"/>
       <c r="B57" s="7"/>
       <c r="C57" s="15" t="s">
-        <v>203</v>
+        <v>254</v>
       </c>
     </row>
     <row r="58" ht="18.75" spans="1:3">
       <c r="A58" s="6"/>
       <c r="B58" s="7"/>
       <c r="C58" s="15" t="s">
-        <v>204</v>
+        <v>255</v>
       </c>
     </row>
     <row r="59" ht="18.75" spans="1:3">
       <c r="A59" s="6"/>
       <c r="B59" s="7"/>
       <c r="C59" s="15" t="s">
-        <v>205</v>
+        <v>256</v>
       </c>
     </row>
     <row r="60" ht="18.75" spans="1:3">
       <c r="A60" s="6"/>
       <c r="B60" s="7"/>
       <c r="C60" s="15" t="s">
-        <v>206</v>
+        <v>257</v>
       </c>
     </row>
     <row r="61" ht="18.75" spans="1:3">
       <c r="A61" s="6"/>
       <c r="B61" s="7"/>
       <c r="C61" s="15" t="s">
-        <v>207</v>
+        <v>258</v>
       </c>
     </row>
     <row r="62" ht="18.75" spans="1:3">
       <c r="A62" s="6"/>
       <c r="B62" s="7"/>
       <c r="C62" s="15" t="s">
-        <v>208</v>
+        <v>259</v>
       </c>
     </row>
     <row r="63" ht="18.75" spans="1:3">
       <c r="A63" s="6"/>
       <c r="B63" s="7"/>
       <c r="C63" s="15" t="s">
-        <v>209</v>
+        <v>260</v>
       </c>
     </row>
     <row r="64" spans="1:3">
@@ -4252,73 +4883,73 @@
     <row r="65" ht="18.75" spans="1:3">
       <c r="A65" s="6"/>
       <c r="B65" s="7" t="s">
-        <v>210</v>
+        <v>261</v>
       </c>
       <c r="C65" s="15" t="s">
-        <v>22</v>
+        <v>74</v>
       </c>
     </row>
     <row r="66" ht="18.75" spans="1:3">
       <c r="A66" s="6"/>
       <c r="B66" s="7"/>
       <c r="C66" s="15" t="s">
-        <v>211</v>
+        <v>262</v>
       </c>
     </row>
     <row r="67" ht="18.75" spans="1:3">
       <c r="A67" s="6"/>
       <c r="B67" s="7"/>
       <c r="C67" s="15" t="s">
-        <v>212</v>
+        <v>263</v>
       </c>
     </row>
     <row r="68" ht="18.75" spans="1:3">
       <c r="A68" s="6"/>
       <c r="B68" s="7"/>
       <c r="C68" s="15" t="s">
-        <v>213</v>
+        <v>264</v>
       </c>
     </row>
     <row r="69" ht="18.75" spans="1:3">
       <c r="A69" s="6"/>
       <c r="B69" s="7"/>
       <c r="C69" s="15" t="s">
-        <v>214</v>
+        <v>265</v>
       </c>
     </row>
     <row r="70" ht="18.75" spans="1:3">
       <c r="A70" s="6"/>
       <c r="B70" s="7"/>
       <c r="C70" s="15" t="s">
-        <v>215</v>
+        <v>266</v>
       </c>
     </row>
     <row r="71" ht="18.75" spans="1:3">
       <c r="A71" s="6"/>
       <c r="B71" s="7"/>
       <c r="C71" s="15" t="s">
-        <v>216</v>
+        <v>267</v>
       </c>
     </row>
     <row r="72" ht="18.75" spans="1:3">
       <c r="A72" s="6"/>
       <c r="B72" s="7"/>
       <c r="C72" s="15" t="s">
-        <v>217</v>
+        <v>268</v>
       </c>
     </row>
     <row r="73" ht="18.75" spans="1:3">
       <c r="A73" s="6"/>
       <c r="B73" s="7"/>
       <c r="C73" s="15" t="s">
-        <v>218</v>
+        <v>269</v>
       </c>
     </row>
     <row r="74" ht="18.75" spans="1:3">
       <c r="A74" s="6"/>
       <c r="B74" s="7"/>
       <c r="C74" s="15" t="s">
-        <v>30</v>
+        <v>82</v>
       </c>
     </row>
     <row r="75" spans="1:3">
@@ -4328,122 +4959,122 @@
     <row r="76" ht="18.75" spans="1:3">
       <c r="A76" s="6"/>
       <c r="B76" s="7" t="s">
-        <v>219</v>
+        <v>270</v>
       </c>
       <c r="C76" s="15" t="s">
-        <v>22</v>
+        <v>74</v>
       </c>
     </row>
     <row r="77" ht="18.75" spans="1:3">
       <c r="A77" s="6"/>
       <c r="B77" s="7"/>
       <c r="C77" s="15" t="s">
-        <v>220</v>
+        <v>271</v>
       </c>
     </row>
     <row r="78" ht="18.75" spans="1:3">
       <c r="A78" s="6"/>
       <c r="B78" s="7"/>
       <c r="C78" s="15" t="s">
-        <v>221</v>
+        <v>272</v>
       </c>
     </row>
     <row r="79" ht="18.75" spans="1:3">
       <c r="A79" s="6"/>
       <c r="B79" s="7"/>
       <c r="C79" s="15" t="s">
-        <v>222</v>
+        <v>273</v>
       </c>
     </row>
     <row r="80" ht="18.75" spans="1:3">
       <c r="A80" s="6"/>
       <c r="B80" s="7"/>
       <c r="C80" s="15" t="s">
-        <v>223</v>
+        <v>274</v>
       </c>
     </row>
     <row r="81" ht="18.75" spans="1:3">
       <c r="A81" s="6"/>
       <c r="B81" s="7"/>
       <c r="C81" s="15" t="s">
-        <v>224</v>
+        <v>275</v>
       </c>
     </row>
     <row r="82" ht="18.75" spans="1:3">
       <c r="A82" s="6"/>
       <c r="B82" s="7"/>
       <c r="C82" s="15" t="s">
-        <v>225</v>
+        <v>276</v>
       </c>
     </row>
     <row r="83" ht="18.75" spans="1:3">
       <c r="A83" s="6"/>
       <c r="B83" s="7"/>
       <c r="C83" s="15" t="s">
-        <v>226</v>
+        <v>277</v>
       </c>
     </row>
     <row r="84" ht="18.75" spans="1:3">
       <c r="A84" s="6"/>
       <c r="B84" s="7"/>
       <c r="C84" s="15" t="s">
-        <v>227</v>
+        <v>278</v>
       </c>
     </row>
     <row r="85" ht="18.75" spans="1:3">
       <c r="A85" s="6"/>
       <c r="B85" s="7"/>
       <c r="C85" s="15" t="s">
-        <v>228</v>
+        <v>279</v>
       </c>
     </row>
     <row r="86" ht="18.75" spans="1:3">
       <c r="A86" s="6"/>
       <c r="B86" s="7"/>
       <c r="C86" s="15" t="s">
-        <v>229</v>
+        <v>280</v>
       </c>
     </row>
     <row r="87" ht="18.75" spans="1:3">
       <c r="A87" s="6"/>
       <c r="B87" s="7"/>
       <c r="C87" s="15" t="s">
-        <v>230</v>
+        <v>281</v>
       </c>
     </row>
     <row r="88" ht="18.75" spans="1:3">
       <c r="A88" s="6"/>
       <c r="B88" s="7"/>
       <c r="C88" s="15" t="s">
-        <v>231</v>
+        <v>282</v>
       </c>
     </row>
     <row r="89" ht="18.75" spans="1:3">
       <c r="A89" s="6"/>
       <c r="B89" s="7"/>
       <c r="C89" s="15" t="s">
-        <v>232</v>
+        <v>283</v>
       </c>
     </row>
     <row r="90" ht="18.75" spans="1:3">
       <c r="A90" s="6"/>
       <c r="B90" s="7"/>
       <c r="C90" s="15" t="s">
-        <v>233</v>
+        <v>284</v>
       </c>
     </row>
     <row r="91" ht="18.75" spans="1:3">
       <c r="A91" s="6"/>
       <c r="B91" s="7"/>
       <c r="C91" s="15" t="s">
-        <v>234</v>
+        <v>285</v>
       </c>
     </row>
     <row r="92" ht="18.75" spans="1:3">
       <c r="A92" s="6"/>
       <c r="B92" s="7"/>
       <c r="C92" s="15" t="s">
-        <v>235</v>
+        <v>286</v>
       </c>
     </row>
     <row r="93" ht="18.75" spans="1:3">
@@ -4454,24 +5085,24 @@
     <row r="94" ht="17" customHeight="1" spans="1:3">
       <c r="A94" s="6"/>
       <c r="B94" s="9" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="C94" s="16" t="s">
-        <v>236</v>
+        <v>287</v>
       </c>
     </row>
     <row r="95" ht="18.75" spans="1:3">
       <c r="A95" s="6"/>
       <c r="B95" s="9"/>
       <c r="C95" s="15" t="s">
-        <v>237</v>
+        <v>288</v>
       </c>
     </row>
     <row r="96" ht="18.75" spans="1:3">
       <c r="A96" s="6"/>
       <c r="B96" s="9"/>
       <c r="C96" s="15" t="s">
-        <v>238</v>
+        <v>289</v>
       </c>
     </row>
     <row r="97" spans="1:3">
@@ -4481,69 +5112,69 @@
     </row>
     <row r="98" ht="24.75" spans="1:3">
       <c r="A98" s="2" t="s">
-        <v>239</v>
+        <v>290</v>
       </c>
       <c r="B98" s="2"/>
       <c r="C98" s="2"/>
     </row>
     <row r="99" ht="18.75" spans="1:3">
       <c r="A99" s="6" t="s">
-        <v>240</v>
+        <v>291</v>
       </c>
       <c r="B99" s="17" t="s">
-        <v>241</v>
+        <v>292</v>
       </c>
       <c r="C99" s="15" t="s">
-        <v>242</v>
+        <v>293</v>
       </c>
     </row>
     <row r="100" ht="18.75" spans="1:3">
       <c r="A100" s="6"/>
       <c r="B100" s="17"/>
       <c r="C100" s="15" t="s">
-        <v>243</v>
+        <v>294</v>
       </c>
     </row>
     <row r="101" ht="18.75" spans="1:3">
       <c r="A101" s="6"/>
       <c r="B101" s="17"/>
       <c r="C101" s="15" t="s">
-        <v>244</v>
+        <v>295</v>
       </c>
     </row>
     <row r="102" ht="18.75" spans="1:3">
       <c r="A102" s="6"/>
       <c r="B102" s="17"/>
       <c r="C102" s="15" t="s">
-        <v>245</v>
+        <v>296</v>
       </c>
     </row>
     <row r="103" ht="18.75" spans="1:3">
       <c r="A103" s="6"/>
       <c r="B103" s="17"/>
       <c r="C103" s="15" t="s">
-        <v>246</v>
+        <v>297</v>
       </c>
     </row>
     <row r="104" ht="18.75" spans="1:3">
       <c r="A104" s="6"/>
       <c r="B104" s="17"/>
       <c r="C104" s="15" t="s">
-        <v>247</v>
+        <v>298</v>
       </c>
     </row>
     <row r="105" ht="18.75" spans="1:3">
       <c r="A105" s="6"/>
       <c r="B105" s="17"/>
       <c r="C105" s="15" t="s">
-        <v>248</v>
+        <v>299</v>
       </c>
     </row>
     <row r="106" ht="18.75" spans="1:3">
       <c r="A106" s="6"/>
       <c r="B106" s="17"/>
       <c r="C106" s="15" t="s">
-        <v>249</v>
+        <v>300</v>
       </c>
     </row>
     <row r="107" spans="1:3">
@@ -4553,108 +5184,108 @@
     <row r="108" ht="18.75" spans="1:3">
       <c r="A108" s="6"/>
       <c r="B108" s="17" t="s">
-        <v>250</v>
+        <v>301</v>
       </c>
       <c r="C108" s="15" t="s">
-        <v>22</v>
+        <v>74</v>
       </c>
     </row>
     <row r="109" ht="18.75" spans="1:3">
       <c r="A109" s="6"/>
       <c r="B109" s="17"/>
       <c r="C109" s="15" t="s">
-        <v>251</v>
+        <v>302</v>
       </c>
     </row>
     <row r="110" ht="18.75" spans="1:3">
       <c r="A110" s="6"/>
       <c r="B110" s="17"/>
       <c r="C110" s="15" t="s">
-        <v>252</v>
+        <v>303</v>
       </c>
     </row>
     <row r="111" ht="18.75" spans="1:3">
       <c r="A111" s="6"/>
       <c r="B111" s="17"/>
       <c r="C111" s="15" t="s">
-        <v>253</v>
+        <v>304</v>
       </c>
     </row>
     <row r="112" ht="18.75" spans="1:3">
       <c r="A112" s="6"/>
       <c r="B112" s="17"/>
       <c r="C112" s="15" t="s">
-        <v>254</v>
+        <v>305</v>
       </c>
     </row>
     <row r="113" ht="18.75" spans="1:3">
       <c r="A113" s="6"/>
       <c r="B113" s="17"/>
       <c r="C113" s="15" t="s">
-        <v>255</v>
+        <v>306</v>
       </c>
     </row>
     <row r="114" ht="18.75" spans="1:3">
       <c r="A114" s="6"/>
       <c r="B114" s="17"/>
       <c r="C114" s="15" t="s">
-        <v>256</v>
+        <v>307</v>
       </c>
     </row>
     <row r="115" ht="18.75" spans="1:3">
       <c r="A115" s="6"/>
       <c r="B115" s="17"/>
       <c r="C115" s="15" t="s">
-        <v>257</v>
+        <v>308</v>
       </c>
     </row>
     <row r="116" ht="18.75" spans="1:3">
       <c r="A116" s="6"/>
       <c r="B116" s="17"/>
       <c r="C116" s="15" t="s">
-        <v>258</v>
+        <v>309</v>
       </c>
     </row>
     <row r="117" ht="18.75" spans="1:3">
       <c r="A117" s="6"/>
       <c r="B117" s="17"/>
       <c r="C117" s="15" t="s">
-        <v>259</v>
+        <v>310</v>
       </c>
     </row>
     <row r="118" ht="18.75" spans="1:3">
       <c r="A118" s="6"/>
       <c r="B118" s="17"/>
       <c r="C118" s="15" t="s">
-        <v>260</v>
+        <v>311</v>
       </c>
     </row>
     <row r="119" ht="37.5" spans="1:3">
       <c r="A119" s="6"/>
       <c r="B119" s="17"/>
       <c r="C119" s="15" t="s">
-        <v>261</v>
+        <v>312</v>
       </c>
     </row>
     <row r="120" ht="18.75" spans="1:3">
       <c r="A120" s="6"/>
       <c r="B120" s="17"/>
       <c r="C120" s="15" t="s">
-        <v>262</v>
+        <v>313</v>
       </c>
     </row>
     <row r="121" ht="18.75" spans="1:3">
       <c r="A121" s="6"/>
       <c r="B121" s="17"/>
       <c r="C121" s="15" t="s">
-        <v>263</v>
+        <v>314</v>
       </c>
     </row>
     <row r="122" ht="18.75" spans="1:3">
       <c r="A122" s="6"/>
       <c r="B122" s="17"/>
       <c r="C122" s="15" t="s">
-        <v>264</v>
+        <v>315</v>
       </c>
     </row>
     <row r="123" spans="1:3">
@@ -4665,17 +5296,17 @@
     <row r="124" ht="37.5" spans="1:3">
       <c r="A124" s="6"/>
       <c r="B124" s="18" t="s">
-        <v>265</v>
+        <v>316</v>
       </c>
       <c r="C124" s="15" t="s">
-        <v>266</v>
+        <v>317</v>
       </c>
     </row>
     <row r="125" ht="18.75" spans="1:3">
       <c r="A125" s="6"/>
       <c r="B125" s="18"/>
       <c r="C125" s="15" t="s">
-        <v>267</v>
+        <v>318</v>
       </c>
     </row>
     <row r="126" spans="1:3">
@@ -4685,7 +5316,7 @@
     </row>
     <row r="130" ht="18.75" spans="1:2">
       <c r="A130" s="19" t="s">
-        <v>268</v>
+        <v>319</v>
       </c>
       <c r="B130" s="20">
         <v>2</v>
@@ -4693,7 +5324,7 @@
     </row>
     <row r="131" ht="18.75" spans="1:2">
       <c r="A131" s="19" t="s">
-        <v>269</v>
+        <v>320</v>
       </c>
       <c r="B131" s="20">
         <v>16</v>
@@ -4722,13 +5353,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
   <dimension ref="A1:C83"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A39" activePane="bottomLeft" state="frozen"/>
       <selection/>
       <selection pane="bottomLeft" activeCell="A30" sqref="A30:C30"/>
     </sheetView>
@@ -4754,14 +5385,14 @@
     </row>
     <row r="2" ht="24.75" spans="1:3">
       <c r="A2" s="2" t="s">
-        <v>270</v>
+        <v>321</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
     </row>
     <row r="3" ht="15.75" spans="1:3">
       <c r="A3" s="3" t="s">
-        <v>271</v>
+        <v>322</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>20</v>
@@ -4778,80 +5409,80 @@
     <row r="5" ht="15" spans="1:3">
       <c r="A5" s="6"/>
       <c r="B5" s="7" t="s">
-        <v>272</v>
+        <v>323</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>22</v>
+        <v>74</v>
       </c>
     </row>
     <row r="6" ht="15" spans="1:3">
       <c r="A6" s="6"/>
       <c r="B6" s="7"/>
       <c r="C6" s="5" t="s">
-        <v>273</v>
+        <v>324</v>
       </c>
     </row>
     <row r="7" ht="15" spans="1:3">
       <c r="A7" s="6"/>
       <c r="B7" s="7"/>
       <c r="C7" s="5" t="s">
-        <v>274</v>
+        <v>325</v>
       </c>
     </row>
     <row r="8" ht="15" spans="1:3">
       <c r="A8" s="6"/>
       <c r="B8" s="7"/>
       <c r="C8" s="5" t="s">
-        <v>275</v>
+        <v>326</v>
       </c>
     </row>
     <row r="9" ht="15" spans="1:3">
       <c r="A9" s="6"/>
       <c r="B9" s="7"/>
       <c r="C9" s="5" t="s">
-        <v>276</v>
+        <v>327</v>
       </c>
     </row>
     <row r="10" ht="15" spans="1:3">
       <c r="A10" s="6"/>
       <c r="B10" s="7"/>
       <c r="C10" s="5" t="s">
-        <v>277</v>
+        <v>328</v>
       </c>
     </row>
     <row r="11" ht="15" spans="1:3">
       <c r="A11" s="6"/>
       <c r="B11" s="7"/>
       <c r="C11" s="5" t="s">
-        <v>278</v>
+        <v>329</v>
       </c>
     </row>
     <row r="12" ht="15" spans="1:3">
       <c r="A12" s="6"/>
       <c r="B12" s="7"/>
       <c r="C12" s="5" t="s">
-        <v>279</v>
+        <v>330</v>
       </c>
     </row>
     <row r="13" ht="15" spans="1:3">
       <c r="A13" s="6"/>
       <c r="B13" s="7"/>
       <c r="C13" s="5" t="s">
-        <v>280</v>
+        <v>331</v>
       </c>
     </row>
     <row r="14" ht="15" spans="1:3">
       <c r="A14" s="6"/>
       <c r="B14" s="7"/>
       <c r="C14" s="5" t="s">
-        <v>281</v>
+        <v>332</v>
       </c>
     </row>
     <row r="15" ht="15" spans="1:3">
       <c r="A15" s="6"/>
       <c r="B15" s="7"/>
       <c r="C15" s="5" t="s">
-        <v>282</v>
+        <v>333</v>
       </c>
     </row>
     <row r="16" ht="15.75" spans="1:3">
@@ -4862,66 +5493,66 @@
     <row r="17" ht="15" spans="1:3">
       <c r="A17" s="6"/>
       <c r="B17" s="7" t="s">
-        <v>283</v>
+        <v>334</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>22</v>
+        <v>74</v>
       </c>
     </row>
     <row r="18" ht="15" spans="1:3">
       <c r="A18" s="6"/>
       <c r="B18" s="7"/>
       <c r="C18" s="5" t="s">
-        <v>284</v>
+        <v>335</v>
       </c>
     </row>
     <row r="19" ht="15" spans="1:3">
       <c r="A19" s="6"/>
       <c r="B19" s="7"/>
       <c r="C19" s="5" t="s">
-        <v>285</v>
+        <v>336</v>
       </c>
     </row>
     <row r="20" ht="15" spans="1:3">
       <c r="A20" s="6"/>
       <c r="B20" s="7"/>
       <c r="C20" s="5" t="s">
-        <v>286</v>
+        <v>337</v>
       </c>
     </row>
     <row r="21" ht="15" spans="1:3">
       <c r="A21" s="6"/>
       <c r="B21" s="7"/>
       <c r="C21" s="5" t="s">
-        <v>287</v>
+        <v>338</v>
       </c>
     </row>
     <row r="22" ht="15" spans="1:3">
       <c r="A22" s="6"/>
       <c r="B22" s="7"/>
       <c r="C22" s="5" t="s">
-        <v>288</v>
+        <v>339</v>
       </c>
     </row>
     <row r="23" ht="15" spans="1:3">
       <c r="A23" s="6"/>
       <c r="B23" s="7"/>
       <c r="C23" s="5" t="s">
-        <v>289</v>
+        <v>340</v>
       </c>
     </row>
     <row r="24" ht="15" spans="1:3">
       <c r="A24" s="6"/>
       <c r="B24" s="7"/>
       <c r="C24" s="5" t="s">
-        <v>290</v>
+        <v>341</v>
       </c>
     </row>
     <row r="25" ht="15" spans="1:3">
       <c r="A25" s="6"/>
       <c r="B25" s="7"/>
       <c r="C25" s="5" t="s">
-        <v>62</v>
+        <v>114</v>
       </c>
     </row>
     <row r="26" spans="1:3">
@@ -4932,17 +5563,17 @@
     <row r="27" ht="15" spans="1:3">
       <c r="A27" s="6"/>
       <c r="B27" s="9" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="C27" s="10" t="s">
-        <v>291</v>
+        <v>342</v>
       </c>
     </row>
     <row r="28" ht="20" customHeight="1" spans="1:3">
       <c r="A28" s="6"/>
       <c r="B28" s="9"/>
       <c r="C28" s="11" t="s">
-        <v>292</v>
+        <v>343</v>
       </c>
     </row>
     <row r="29" ht="8" customHeight="1" spans="1:3">
@@ -4952,83 +5583,83 @@
     </row>
     <row r="30" customFormat="1" ht="24.75" spans="1:3">
       <c r="A30" s="2" t="s">
-        <v>293</v>
+        <v>344</v>
       </c>
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
     </row>
     <row r="31" ht="15" spans="1:3">
       <c r="A31" s="13" t="s">
-        <v>294</v>
+        <v>345</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>295</v>
+        <v>346</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>22</v>
+        <v>74</v>
       </c>
     </row>
     <row r="32" ht="15" spans="1:3">
       <c r="A32" s="13"/>
       <c r="B32" s="7"/>
       <c r="C32" s="5" t="s">
-        <v>296</v>
+        <v>347</v>
       </c>
     </row>
     <row r="33" ht="15" spans="1:3">
       <c r="A33" s="13"/>
       <c r="B33" s="7"/>
       <c r="C33" s="5" t="s">
-        <v>297</v>
+        <v>348</v>
       </c>
     </row>
     <row r="34" ht="15" spans="1:3">
       <c r="A34" s="13"/>
       <c r="B34" s="7"/>
       <c r="C34" s="5" t="s">
-        <v>298</v>
+        <v>349</v>
       </c>
     </row>
     <row r="35" ht="15" spans="1:3">
       <c r="A35" s="13"/>
       <c r="B35" s="7"/>
       <c r="C35" s="5" t="s">
-        <v>299</v>
+        <v>350</v>
       </c>
     </row>
     <row r="36" ht="15" spans="1:3">
       <c r="A36" s="13"/>
       <c r="B36" s="7"/>
       <c r="C36" s="5" t="s">
-        <v>300</v>
+        <v>351</v>
       </c>
     </row>
     <row r="37" ht="15" spans="1:3">
       <c r="A37" s="13"/>
       <c r="B37" s="7"/>
       <c r="C37" s="5" t="s">
-        <v>301</v>
+        <v>352</v>
       </c>
     </row>
     <row r="38" ht="15" spans="1:3">
       <c r="A38" s="13"/>
       <c r="B38" s="7"/>
       <c r="C38" s="5" t="s">
-        <v>302</v>
+        <v>353</v>
       </c>
     </row>
     <row r="39" ht="15" spans="1:3">
       <c r="A39" s="13"/>
       <c r="B39" s="7"/>
       <c r="C39" s="5" t="s">
-        <v>303</v>
+        <v>354</v>
       </c>
     </row>
     <row r="40" ht="15" spans="1:3">
       <c r="A40" s="13"/>
       <c r="B40" s="7"/>
       <c r="C40" s="5" t="s">
-        <v>30</v>
+        <v>82</v>
       </c>
     </row>
     <row r="41" ht="15.75" spans="1:3">
@@ -5039,103 +5670,103 @@
     <row r="42" ht="15" spans="1:3">
       <c r="A42" s="13"/>
       <c r="B42" s="7" t="s">
-        <v>304</v>
+        <v>355</v>
       </c>
       <c r="C42" s="5" t="s">
-        <v>22</v>
+        <v>74</v>
       </c>
     </row>
     <row r="43" ht="15" spans="1:3">
       <c r="A43" s="13"/>
       <c r="B43" s="7"/>
       <c r="C43" s="5" t="s">
-        <v>305</v>
+        <v>356</v>
       </c>
     </row>
     <row r="44" ht="15" spans="1:3">
       <c r="A44" s="13"/>
       <c r="B44" s="7"/>
       <c r="C44" s="5" t="s">
-        <v>306</v>
+        <v>357</v>
       </c>
     </row>
     <row r="45" ht="15" spans="1:3">
       <c r="A45" s="13"/>
       <c r="B45" s="7"/>
       <c r="C45" s="5" t="s">
-        <v>307</v>
+        <v>358</v>
       </c>
     </row>
     <row r="46" ht="15" spans="1:3">
       <c r="A46" s="13"/>
       <c r="B46" s="7"/>
       <c r="C46" s="5" t="s">
-        <v>308</v>
+        <v>359</v>
       </c>
     </row>
     <row r="47" ht="15" spans="1:3">
       <c r="A47" s="13"/>
       <c r="B47" s="7"/>
       <c r="C47" s="5" t="s">
-        <v>309</v>
+        <v>360</v>
       </c>
     </row>
     <row r="48" ht="15" spans="1:3">
       <c r="A48" s="13"/>
       <c r="B48" s="7"/>
       <c r="C48" s="5" t="s">
-        <v>310</v>
+        <v>361</v>
       </c>
     </row>
     <row r="49" ht="15" spans="1:3">
       <c r="A49" s="13"/>
       <c r="B49" s="7"/>
       <c r="C49" s="5" t="s">
-        <v>311</v>
+        <v>362</v>
       </c>
     </row>
     <row r="50" ht="15" spans="1:3">
       <c r="A50" s="13"/>
       <c r="B50" s="7"/>
       <c r="C50" s="5" t="s">
-        <v>312</v>
+        <v>363</v>
       </c>
     </row>
     <row r="51" spans="1:3">
       <c r="A51" s="13"/>
       <c r="B51" s="7"/>
       <c r="C51" s="8" t="s">
-        <v>313</v>
+        <v>364</v>
       </c>
     </row>
     <row r="52" spans="1:3">
       <c r="A52" s="13"/>
       <c r="B52" s="7"/>
       <c r="C52" s="8" t="s">
-        <v>314</v>
+        <v>365</v>
       </c>
     </row>
     <row r="53" spans="1:3">
       <c r="A53" s="13"/>
       <c r="B53" s="7"/>
       <c r="C53" s="8" t="s">
-        <v>191</v>
+        <v>242</v>
       </c>
     </row>
     <row r="54" ht="15" spans="1:3">
       <c r="A54" s="13"/>
       <c r="B54" s="9" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="C54" s="10" t="s">
-        <v>291</v>
+        <v>342</v>
       </c>
     </row>
     <row r="55" ht="15" spans="1:3">
       <c r="A55" s="13"/>
       <c r="B55" s="9"/>
       <c r="C55" s="11" t="s">
-        <v>315</v>
+        <v>366</v>
       </c>
     </row>
     <row r="56" customFormat="1" ht="9" customHeight="1" spans="1:3">

</xml_diff>

<commit_message>
Added Course Materials - Day 6.
</commit_message>
<xml_diff>
--- a/JEE DevOps - TOC.xlsx
+++ b/JEE DevOps - TOC.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20490" windowHeight="7815" activeTab="3"/>
+    <workbookView windowWidth="20490" windowHeight="7815" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="7" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="461" uniqueCount="383">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="456" uniqueCount="377">
   <si>
     <t>Sr. No.</t>
   </si>
@@ -875,49 +875,40 @@
     <t>3. Database Overview</t>
   </si>
   <si>
-    <t>4.  MySQL Setup and Installation</t>
-  </si>
-  <si>
-    <t>5. persistence.xml</t>
-  </si>
-  <si>
-    <t>6. persistence.xml Demo</t>
-  </si>
-  <si>
-    <t>7. pom.xml</t>
-  </si>
-  <si>
-    <t>8. pom.xml Demo</t>
-  </si>
-  <si>
-    <t>9. jpaContext.xml</t>
-  </si>
-  <si>
-    <t>10. jpaContext.xml Demo</t>
-  </si>
-  <si>
-    <t>11. Entity Manager Factory</t>
-  </si>
-  <si>
-    <t>12. Adding MySql Dependency</t>
-  </si>
-  <si>
-    <t>13. MySQL Maven Demo</t>
-  </si>
-  <si>
-    <t>14. application.properties Demo</t>
-  </si>
-  <si>
-    <t>15. Transactional</t>
-  </si>
-  <si>
-    <t>16. Tips and Tricks</t>
-  </si>
-  <si>
-    <t>17. Logging Configuration</t>
-  </si>
-  <si>
-    <t>18. Summary</t>
+    <t>4. PostgreSQL Setup and Installation</t>
+  </si>
+  <si>
+    <t>5. pom.xml</t>
+  </si>
+  <si>
+    <t>6. pom.xml Demo</t>
+  </si>
+  <si>
+    <t>7. jpaContext.xml</t>
+  </si>
+  <si>
+    <t>8. Entity Manager Factory</t>
+  </si>
+  <si>
+    <t>9. Adding PostgreSQL Dependency</t>
+  </si>
+  <si>
+    <t>10. PostgreSQL  Maven Demo</t>
+  </si>
+  <si>
+    <t>11. application.properties Demo</t>
+  </si>
+  <si>
+    <t>12. Transactional</t>
+  </si>
+  <si>
+    <t>13. Tips and Tricks</t>
+  </si>
+  <si>
+    <t>14. Logging Configuration</t>
+  </si>
+  <si>
+    <t>15. Summary</t>
   </si>
   <si>
     <t>7. Overview of JPA and Creating Your First Entity</t>
@@ -938,13 +929,7 @@
     <t>6. Verify Database Demo</t>
   </si>
   <si>
-    <t>7. MySQL Workbench Download</t>
-  </si>
-  <si>
-    <t>8. MySQL Workbench Demo</t>
-  </si>
-  <si>
-    <t>9. Run the App and Verify Tables Demo</t>
+    <t>7. Run the App and Verify Tables Demo</t>
   </si>
   <si>
     <t>8. JPA Annotations and How to Use Them</t>
@@ -1080,9 +1065,6 @@
   </si>
   <si>
     <t>14. Spring Data JPA Recap</t>
-  </si>
-  <si>
-    <t>15. Summary</t>
   </si>
   <si>
     <t>Hand On Assignments</t>
@@ -1291,10 +1273,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="40">
     <font>
@@ -1442,41 +1424,32 @@
       <charset val="134"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="3"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <sz val="13"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1503,8 +1476,30 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="13"/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -1519,25 +1514,34 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1557,30 +1561,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1619,7 +1601,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1631,7 +1655,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1643,97 +1703,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1751,7 +1721,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1763,13 +1745,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1781,25 +1769,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1893,41 +1875,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
       <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1952,6 +1904,45 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1981,27 +1972,18 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="24" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="42" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -2011,130 +1993,130 @@
     <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="7" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="14" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="11" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="18" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="25" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="36" fillId="25" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="13" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="18" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="18" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="38" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="39" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="37" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -3767,8 +3749,8 @@
   <sheetPr/>
   <dimension ref="A1:C72"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A43" activePane="bottomLeft" state="frozen"/>
       <selection/>
       <selection pane="bottomLeft" activeCell="C35" sqref="C35"/>
     </sheetView>
@@ -4534,12 +4516,12 @@
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:C131"/>
+  <dimension ref="A1:C126"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A116" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A58" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="A98" sqref="A98:C98"/>
+      <selection pane="bottomLeft" activeCell="F59" sqref="F59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" outlineLevelCol="2"/>
@@ -4975,38 +4957,38 @@
         <v>264</v>
       </c>
     </row>
-    <row r="61" ht="18.75" spans="1:3">
+    <row r="61" spans="1:3">
       <c r="A61" s="10"/>
-      <c r="B61" s="11"/>
-      <c r="C61" s="19" t="s">
-        <v>265</v>
-      </c>
+      <c r="C61" s="12"/>
     </row>
     <row r="62" ht="18.75" spans="1:3">
       <c r="A62" s="10"/>
-      <c r="B62" s="11"/>
+      <c r="B62" s="11" t="s">
+        <v>265</v>
+      </c>
       <c r="C62" s="19" t="s">
-        <v>266</v>
+        <v>74</v>
       </c>
     </row>
     <row r="63" ht="18.75" spans="1:3">
       <c r="A63" s="10"/>
       <c r="B63" s="11"/>
       <c r="C63" s="19" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="64" ht="18.75" spans="1:3">
+      <c r="A64" s="10"/>
+      <c r="B64" s="11"/>
+      <c r="C64" s="19" t="s">
         <v>267</v>
       </c>
-    </row>
-    <row r="64" spans="1:3">
-      <c r="A64" s="10"/>
-      <c r="C64" s="12"/>
     </row>
     <row r="65" ht="18.75" spans="1:3">
       <c r="A65" s="10"/>
-      <c r="B65" s="11" t="s">
+      <c r="B65" s="11"/>
+      <c r="C65" s="19" t="s">
         <v>268</v>
-      </c>
-      <c r="C65" s="19" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="66" ht="18.75" spans="1:3">
@@ -5034,55 +5016,55 @@
       <c r="A69" s="10"/>
       <c r="B69" s="11"/>
       <c r="C69" s="19" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="70" ht="18.75" spans="1:3">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3">
       <c r="A70" s="10"/>
-      <c r="B70" s="11"/>
-      <c r="C70" s="19" t="s">
-        <v>273</v>
-      </c>
+      <c r="C70" s="12"/>
     </row>
     <row r="71" ht="18.75" spans="1:3">
       <c r="A71" s="10"/>
-      <c r="B71" s="11"/>
+      <c r="B71" s="11" t="s">
+        <v>272</v>
+      </c>
       <c r="C71" s="19" t="s">
-        <v>274</v>
+        <v>74</v>
       </c>
     </row>
     <row r="72" ht="18.75" spans="1:3">
       <c r="A72" s="10"/>
       <c r="B72" s="11"/>
       <c r="C72" s="19" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
     </row>
     <row r="73" ht="18.75" spans="1:3">
       <c r="A73" s="10"/>
       <c r="B73" s="11"/>
       <c r="C73" s="19" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
     </row>
     <row r="74" ht="18.75" spans="1:3">
       <c r="A74" s="10"/>
       <c r="B74" s="11"/>
       <c r="C74" s="19" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="75" ht="18.75" spans="1:3">
       <c r="A75" s="10"/>
-      <c r="C75" s="12"/>
+      <c r="B75" s="11"/>
+      <c r="C75" s="19" t="s">
+        <v>276</v>
+      </c>
     </row>
     <row r="76" ht="18.75" spans="1:3">
       <c r="A76" s="10"/>
-      <c r="B76" s="11" t="s">
+      <c r="B76" s="11"/>
+      <c r="C76" s="19" t="s">
         <v>277</v>
-      </c>
-      <c r="C76" s="19" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="77" ht="18.75" spans="1:3">
@@ -5165,85 +5147,85 @@
     <row r="88" ht="18.75" spans="1:3">
       <c r="A88" s="10"/>
       <c r="B88" s="11"/>
-      <c r="C88" s="19" t="s">
+      <c r="C88" s="19"/>
+    </row>
+    <row r="89" ht="17" customHeight="1" spans="1:3">
+      <c r="A89" s="10"/>
+      <c r="B89" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="C89" s="20" t="s">
         <v>289</v>
-      </c>
-    </row>
-    <row r="89" ht="18.75" spans="1:3">
-      <c r="A89" s="10"/>
-      <c r="B89" s="11"/>
-      <c r="C89" s="19" t="s">
-        <v>290</v>
       </c>
     </row>
     <row r="90" ht="18.75" spans="1:3">
       <c r="A90" s="10"/>
-      <c r="B90" s="11"/>
+      <c r="B90" s="13"/>
       <c r="C90" s="19" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="91" ht="18.75" spans="1:3">
       <c r="A91" s="10"/>
-      <c r="B91" s="11"/>
+      <c r="B91" s="13"/>
       <c r="C91" s="19" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3">
+      <c r="A92" s="16"/>
+      <c r="B92" s="16"/>
+      <c r="C92" s="16"/>
+    </row>
+    <row r="93" ht="24.75" spans="1:3">
+      <c r="A93" s="1" t="s">
         <v>292</v>
       </c>
-    </row>
-    <row r="92" ht="18.75" spans="1:3">
-      <c r="A92" s="10"/>
-      <c r="B92" s="11"/>
-      <c r="C92" s="19" t="s">
+      <c r="B93" s="1"/>
+      <c r="C93" s="1"/>
+    </row>
+    <row r="94" ht="18.75" spans="1:3">
+      <c r="A94" s="10" t="s">
         <v>293</v>
       </c>
-    </row>
-    <row r="93" ht="18.75" spans="1:3">
-      <c r="A93" s="10"/>
-      <c r="B93" s="11"/>
-      <c r="C93" s="19"/>
-    </row>
-    <row r="94" ht="17" customHeight="1" spans="1:3">
-      <c r="A94" s="10"/>
-      <c r="B94" s="13" t="s">
-        <v>66</v>
-      </c>
-      <c r="C94" s="20" t="s">
+      <c r="B94" s="21" t="s">
         <v>294</v>
+      </c>
+      <c r="C94" s="19" t="s">
+        <v>295</v>
       </c>
     </row>
     <row r="95" ht="18.75" spans="1:3">
       <c r="A95" s="10"/>
-      <c r="B95" s="13"/>
+      <c r="B95" s="21"/>
       <c r="C95" s="19" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
     </row>
     <row r="96" ht="18.75" spans="1:3">
       <c r="A96" s="10"/>
-      <c r="B96" s="13"/>
+      <c r="B96" s="21"/>
       <c r="C96" s="19" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="97" spans="1:3">
-      <c r="A97" s="16"/>
-      <c r="B97" s="16"/>
-      <c r="C97" s="16"/>
-    </row>
-    <row r="98" ht="24.75" spans="1:3">
-      <c r="A98" s="1" t="s">
         <v>297</v>
       </c>
-      <c r="B98" s="1"/>
-      <c r="C98" s="1"/>
+    </row>
+    <row r="97" ht="18.75" spans="1:3">
+      <c r="A97" s="10"/>
+      <c r="B97" s="21"/>
+      <c r="C97" s="19" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="98" ht="18.75" spans="1:3">
+      <c r="A98" s="10"/>
+      <c r="B98" s="21"/>
+      <c r="C98" s="19" t="s">
+        <v>299</v>
+      </c>
     </row>
     <row r="99" ht="18.75" spans="1:3">
-      <c r="A99" s="10" t="s">
-        <v>298</v>
-      </c>
-      <c r="B99" s="21" t="s">
-        <v>299</v>
-      </c>
+      <c r="A99" s="10"/>
+      <c r="B99" s="21"/>
       <c r="C99" s="19" t="s">
         <v>300</v>
       </c>
@@ -5262,52 +5244,52 @@
         <v>302</v>
       </c>
     </row>
-    <row r="102" ht="18.75" spans="1:3">
+    <row r="102" spans="1:3">
       <c r="A102" s="10"/>
-      <c r="B102" s="21"/>
-      <c r="C102" s="19" t="s">
-        <v>303</v>
-      </c>
+      <c r="C102" s="12"/>
     </row>
     <row r="103" ht="18.75" spans="1:3">
       <c r="A103" s="10"/>
-      <c r="B103" s="21"/>
+      <c r="B103" s="21" t="s">
+        <v>303</v>
+      </c>
       <c r="C103" s="19" t="s">
-        <v>304</v>
+        <v>74</v>
       </c>
     </row>
     <row r="104" ht="18.75" spans="1:3">
       <c r="A104" s="10"/>
       <c r="B104" s="21"/>
       <c r="C104" s="19" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="105" ht="18.75" spans="1:3">
       <c r="A105" s="10"/>
       <c r="B105" s="21"/>
       <c r="C105" s="19" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="106" ht="18.75" spans="1:3">
       <c r="A106" s="10"/>
       <c r="B106" s="21"/>
       <c r="C106" s="19" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="107" ht="18.75" spans="1:3">
+      <c r="A107" s="10"/>
+      <c r="B107" s="21"/>
+      <c r="C107" s="19" t="s">
         <v>307</v>
       </c>
-    </row>
-    <row r="107" spans="1:3">
-      <c r="A107" s="10"/>
-      <c r="C107" s="12"/>
     </row>
     <row r="108" ht="18.75" spans="1:3">
       <c r="A108" s="10"/>
-      <c r="B108" s="21" t="s">
+      <c r="B108" s="21"/>
+      <c r="C108" s="19" t="s">
         <v>308</v>
-      </c>
-      <c r="C108" s="19" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="109" ht="18.75" spans="1:3">
@@ -5345,7 +5327,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="114" ht="18.75" spans="1:3">
+    <row r="114" ht="37.5" spans="1:3">
       <c r="A114" s="10"/>
       <c r="B114" s="21"/>
       <c r="C114" s="19" t="s">
@@ -5370,103 +5352,68 @@
       <c r="A117" s="10"/>
       <c r="B117" s="21"/>
       <c r="C117" s="19" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="118" ht="18.75" spans="1:3">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3">
       <c r="A118" s="10"/>
-      <c r="B118" s="21"/>
-      <c r="C118" s="19" t="s">
-        <v>318</v>
-      </c>
+      <c r="B118" s="12"/>
+      <c r="C118" s="12"/>
     </row>
     <row r="119" ht="37.5" spans="1:3">
       <c r="A119" s="10"/>
-      <c r="B119" s="21"/>
+      <c r="B119" s="22" t="s">
+        <v>317</v>
+      </c>
       <c r="C119" s="19" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="120" ht="18.75" spans="1:3">
       <c r="A120" s="10"/>
-      <c r="B120" s="21"/>
+      <c r="B120" s="22"/>
       <c r="C120" s="19" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3">
+      <c r="A121" s="16"/>
+      <c r="B121" s="16"/>
+      <c r="C121" s="16"/>
+    </row>
+    <row r="125" ht="18.75" spans="1:2">
+      <c r="A125" s="23" t="s">
         <v>320</v>
       </c>
-    </row>
-    <row r="121" ht="18.75" spans="1:3">
-      <c r="A121" s="10"/>
-      <c r="B121" s="21"/>
-      <c r="C121" s="19" t="s">
+      <c r="B125" s="24">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="126" ht="18.75" spans="1:2">
+      <c r="A126" s="23" t="s">
         <v>321</v>
       </c>
-    </row>
-    <row r="122" ht="18.75" spans="1:3">
-      <c r="A122" s="10"/>
-      <c r="B122" s="21"/>
-      <c r="C122" s="19" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="123" spans="1:3">
-      <c r="A123" s="10"/>
-      <c r="B123" s="12"/>
-      <c r="C123" s="12"/>
-    </row>
-    <row r="124" ht="37.5" spans="1:3">
-      <c r="A124" s="10"/>
-      <c r="B124" s="22" t="s">
-        <v>323</v>
-      </c>
-      <c r="C124" s="19" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="125" ht="18.75" spans="1:3">
-      <c r="A125" s="10"/>
-      <c r="B125" s="22"/>
-      <c r="C125" s="19" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="126" spans="1:3">
-      <c r="A126" s="16"/>
-      <c r="B126" s="16"/>
-      <c r="C126" s="16"/>
-    </row>
-    <row r="130" ht="18.75" spans="1:2">
-      <c r="A130" s="23" t="s">
-        <v>326</v>
-      </c>
-      <c r="B130" s="24">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="131" ht="18.75" spans="1:2">
-      <c r="A131" s="23" t="s">
-        <v>327</v>
-      </c>
-      <c r="B131" s="24">
+      <c r="B126" s="24">
         <v>16</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="15">
     <mergeCell ref="A2:C2"/>
-    <mergeCell ref="A98:C98"/>
-    <mergeCell ref="A3:A96"/>
-    <mergeCell ref="A99:A125"/>
+    <mergeCell ref="A93:C93"/>
+    <mergeCell ref="A3:A91"/>
+    <mergeCell ref="A94:A120"/>
     <mergeCell ref="B5:B11"/>
     <mergeCell ref="B13:B21"/>
     <mergeCell ref="B23:B32"/>
     <mergeCell ref="B33:B44"/>
-    <mergeCell ref="B46:B63"/>
-    <mergeCell ref="B65:B74"/>
-    <mergeCell ref="B76:B92"/>
-    <mergeCell ref="B94:B96"/>
-    <mergeCell ref="B99:B106"/>
-    <mergeCell ref="B108:B122"/>
-    <mergeCell ref="B124:B125"/>
+    <mergeCell ref="B46:B60"/>
+    <mergeCell ref="B62:B69"/>
+    <mergeCell ref="B71:B87"/>
+    <mergeCell ref="B89:B91"/>
+    <mergeCell ref="B94:B101"/>
+    <mergeCell ref="B103:B117"/>
+    <mergeCell ref="B119:B120"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>
@@ -5505,14 +5452,14 @@
     </row>
     <row r="2" ht="24.75" spans="1:3">
       <c r="A2" s="1" t="s">
-        <v>328</v>
+        <v>322</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
     </row>
     <row r="3" ht="15.75" spans="1:3">
       <c r="A3" s="7" t="s">
-        <v>329</v>
+        <v>323</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>20</v>
@@ -5529,7 +5476,7 @@
     <row r="5" ht="15" spans="1:3">
       <c r="A5" s="10"/>
       <c r="B5" s="11" t="s">
-        <v>330</v>
+        <v>324</v>
       </c>
       <c r="C5" s="9" t="s">
         <v>74</v>
@@ -5539,70 +5486,70 @@
       <c r="A6" s="10"/>
       <c r="B6" s="11"/>
       <c r="C6" s="9" t="s">
-        <v>331</v>
+        <v>325</v>
       </c>
     </row>
     <row r="7" ht="15" spans="1:3">
       <c r="A7" s="10"/>
       <c r="B7" s="11"/>
       <c r="C7" s="9" t="s">
-        <v>332</v>
+        <v>326</v>
       </c>
     </row>
     <row r="8" ht="15" spans="1:3">
       <c r="A8" s="10"/>
       <c r="B8" s="11"/>
       <c r="C8" s="9" t="s">
-        <v>333</v>
+        <v>327</v>
       </c>
     </row>
     <row r="9" ht="15" spans="1:3">
       <c r="A9" s="10"/>
       <c r="B9" s="11"/>
       <c r="C9" s="9" t="s">
-        <v>334</v>
+        <v>328</v>
       </c>
     </row>
     <row r="10" ht="15" spans="1:3">
       <c r="A10" s="10"/>
       <c r="B10" s="11"/>
       <c r="C10" s="9" t="s">
-        <v>335</v>
+        <v>329</v>
       </c>
     </row>
     <row r="11" ht="15" spans="1:3">
       <c r="A11" s="10"/>
       <c r="B11" s="11"/>
       <c r="C11" s="9" t="s">
-        <v>336</v>
+        <v>330</v>
       </c>
     </row>
     <row r="12" ht="15" spans="1:3">
       <c r="A12" s="10"/>
       <c r="B12" s="11"/>
       <c r="C12" s="9" t="s">
-        <v>337</v>
+        <v>331</v>
       </c>
     </row>
     <row r="13" ht="15" spans="1:3">
       <c r="A13" s="10"/>
       <c r="B13" s="11"/>
       <c r="C13" s="9" t="s">
-        <v>338</v>
+        <v>332</v>
       </c>
     </row>
     <row r="14" ht="15" spans="1:3">
       <c r="A14" s="10"/>
       <c r="B14" s="11"/>
       <c r="C14" s="9" t="s">
-        <v>339</v>
+        <v>333</v>
       </c>
     </row>
     <row r="15" ht="15" spans="1:3">
       <c r="A15" s="10"/>
       <c r="B15" s="11"/>
       <c r="C15" s="9" t="s">
-        <v>340</v>
+        <v>334</v>
       </c>
     </row>
     <row r="16" ht="15.75" spans="1:3">
@@ -5613,7 +5560,7 @@
     <row r="17" ht="15" spans="1:3">
       <c r="A17" s="10"/>
       <c r="B17" s="11" t="s">
-        <v>341</v>
+        <v>335</v>
       </c>
       <c r="C17" s="9" t="s">
         <v>74</v>
@@ -5623,49 +5570,49 @@
       <c r="A18" s="10"/>
       <c r="B18" s="11"/>
       <c r="C18" s="9" t="s">
-        <v>342</v>
+        <v>336</v>
       </c>
     </row>
     <row r="19" ht="15" spans="1:3">
       <c r="A19" s="10"/>
       <c r="B19" s="11"/>
       <c r="C19" s="9" t="s">
-        <v>343</v>
+        <v>337</v>
       </c>
     </row>
     <row r="20" ht="15" spans="1:3">
       <c r="A20" s="10"/>
       <c r="B20" s="11"/>
       <c r="C20" s="9" t="s">
-        <v>344</v>
+        <v>338</v>
       </c>
     </row>
     <row r="21" ht="15" spans="1:3">
       <c r="A21" s="10"/>
       <c r="B21" s="11"/>
       <c r="C21" s="9" t="s">
-        <v>345</v>
+        <v>339</v>
       </c>
     </row>
     <row r="22" ht="15" spans="1:3">
       <c r="A22" s="10"/>
       <c r="B22" s="11"/>
       <c r="C22" s="9" t="s">
-        <v>346</v>
+        <v>340</v>
       </c>
     </row>
     <row r="23" ht="15" spans="1:3">
       <c r="A23" s="10"/>
       <c r="B23" s="11"/>
       <c r="C23" s="9" t="s">
-        <v>347</v>
+        <v>341</v>
       </c>
     </row>
     <row r="24" ht="15" spans="1:3">
       <c r="A24" s="10"/>
       <c r="B24" s="11"/>
       <c r="C24" s="9" t="s">
-        <v>348</v>
+        <v>342</v>
       </c>
     </row>
     <row r="25" ht="15" spans="1:3">
@@ -5686,14 +5633,14 @@
         <v>66</v>
       </c>
       <c r="C27" s="14" t="s">
-        <v>349</v>
+        <v>343</v>
       </c>
     </row>
     <row r="28" ht="20" customHeight="1" spans="1:3">
       <c r="A28" s="10"/>
       <c r="B28" s="13"/>
       <c r="C28" s="15" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
     </row>
     <row r="29" ht="8" customHeight="1" spans="1:3">
@@ -5703,17 +5650,17 @@
     </row>
     <row r="30" customFormat="1" ht="24.75" spans="1:3">
       <c r="A30" s="1" t="s">
-        <v>351</v>
+        <v>345</v>
       </c>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
     </row>
     <row r="31" ht="15" spans="1:3">
       <c r="A31" s="17" t="s">
-        <v>352</v>
+        <v>346</v>
       </c>
       <c r="B31" s="11" t="s">
-        <v>353</v>
+        <v>347</v>
       </c>
       <c r="C31" s="9" t="s">
         <v>74</v>
@@ -5723,56 +5670,56 @@
       <c r="A32" s="17"/>
       <c r="B32" s="11"/>
       <c r="C32" s="9" t="s">
-        <v>354</v>
+        <v>348</v>
       </c>
     </row>
     <row r="33" ht="15" spans="1:3">
       <c r="A33" s="17"/>
       <c r="B33" s="11"/>
       <c r="C33" s="9" t="s">
-        <v>355</v>
+        <v>349</v>
       </c>
     </row>
     <row r="34" ht="15" spans="1:3">
       <c r="A34" s="17"/>
       <c r="B34" s="11"/>
       <c r="C34" s="9" t="s">
-        <v>356</v>
+        <v>350</v>
       </c>
     </row>
     <row r="35" ht="15" spans="1:3">
       <c r="A35" s="17"/>
       <c r="B35" s="11"/>
       <c r="C35" s="9" t="s">
-        <v>357</v>
+        <v>351</v>
       </c>
     </row>
     <row r="36" ht="15" spans="1:3">
       <c r="A36" s="17"/>
       <c r="B36" s="11"/>
       <c r="C36" s="9" t="s">
-        <v>358</v>
+        <v>352</v>
       </c>
     </row>
     <row r="37" ht="15" spans="1:3">
       <c r="A37" s="17"/>
       <c r="B37" s="11"/>
       <c r="C37" s="9" t="s">
-        <v>359</v>
+        <v>353</v>
       </c>
     </row>
     <row r="38" ht="15" spans="1:3">
       <c r="A38" s="17"/>
       <c r="B38" s="11"/>
       <c r="C38" s="9" t="s">
-        <v>360</v>
+        <v>354</v>
       </c>
     </row>
     <row r="39" ht="15" spans="1:3">
       <c r="A39" s="17"/>
       <c r="B39" s="11"/>
       <c r="C39" s="9" t="s">
-        <v>361</v>
+        <v>355</v>
       </c>
     </row>
     <row r="40" ht="15" spans="1:3">
@@ -5790,7 +5737,7 @@
     <row r="42" ht="15" spans="1:3">
       <c r="A42" s="17"/>
       <c r="B42" s="11" t="s">
-        <v>362</v>
+        <v>356</v>
       </c>
       <c r="C42" s="9" t="s">
         <v>74</v>
@@ -5800,70 +5747,70 @@
       <c r="A43" s="17"/>
       <c r="B43" s="11"/>
       <c r="C43" s="9" t="s">
-        <v>363</v>
+        <v>357</v>
       </c>
     </row>
     <row r="44" ht="15" spans="1:3">
       <c r="A44" s="17"/>
       <c r="B44" s="11"/>
       <c r="C44" s="9" t="s">
-        <v>364</v>
+        <v>358</v>
       </c>
     </row>
     <row r="45" ht="15" spans="1:3">
       <c r="A45" s="17"/>
       <c r="B45" s="11"/>
       <c r="C45" s="9" t="s">
-        <v>365</v>
+        <v>359</v>
       </c>
     </row>
     <row r="46" ht="15" spans="1:3">
       <c r="A46" s="17"/>
       <c r="B46" s="11"/>
       <c r="C46" s="9" t="s">
-        <v>366</v>
+        <v>360</v>
       </c>
     </row>
     <row r="47" ht="15" spans="1:3">
       <c r="A47" s="17"/>
       <c r="B47" s="11"/>
       <c r="C47" s="9" t="s">
-        <v>367</v>
+        <v>361</v>
       </c>
     </row>
     <row r="48" ht="15" spans="1:3">
       <c r="A48" s="17"/>
       <c r="B48" s="11"/>
       <c r="C48" s="9" t="s">
-        <v>368</v>
+        <v>362</v>
       </c>
     </row>
     <row r="49" ht="15" spans="1:3">
       <c r="A49" s="17"/>
       <c r="B49" s="11"/>
       <c r="C49" s="9" t="s">
-        <v>369</v>
+        <v>363</v>
       </c>
     </row>
     <row r="50" ht="15" spans="1:3">
       <c r="A50" s="17"/>
       <c r="B50" s="11"/>
       <c r="C50" s="9" t="s">
-        <v>370</v>
+        <v>364</v>
       </c>
     </row>
     <row r="51" spans="1:3">
       <c r="A51" s="17"/>
       <c r="B51" s="11"/>
       <c r="C51" s="12" t="s">
-        <v>371</v>
+        <v>365</v>
       </c>
     </row>
     <row r="52" spans="1:3">
       <c r="A52" s="17"/>
       <c r="B52" s="11"/>
       <c r="C52" s="12" t="s">
-        <v>372</v>
+        <v>366</v>
       </c>
     </row>
     <row r="53" spans="1:3">
@@ -5879,14 +5826,14 @@
         <v>66</v>
       </c>
       <c r="C54" s="14" t="s">
-        <v>349</v>
+        <v>343</v>
       </c>
     </row>
     <row r="55" ht="15" spans="1:3">
       <c r="A55" s="17"/>
       <c r="B55" s="13"/>
       <c r="C55" s="15" t="s">
-        <v>373</v>
+        <v>367</v>
       </c>
     </row>
     <row r="56" customFormat="1" ht="9" customHeight="1" spans="1:3">
@@ -6015,7 +5962,7 @@
   <sheetData>
     <row r="1" customFormat="1" ht="24.75" spans="1:4">
       <c r="A1" s="1" t="s">
-        <v>351</v>
+        <v>345</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -6023,16 +5970,16 @@
     </row>
     <row r="2" ht="15" spans="1:4">
       <c r="A2" s="2" t="s">
-        <v>374</v>
+        <v>368</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>375</v>
+        <v>369</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>376</v>
+        <v>370</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>377</v>
+        <v>371</v>
       </c>
     </row>
     <row r="4" ht="25.5" spans="1:4">
@@ -6040,10 +5987,10 @@
         <v>1</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>378</v>
+        <v>372</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>379</v>
+        <v>373</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>68</v>
@@ -6054,13 +6001,13 @@
         <v>2</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>380</v>
+        <v>374</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>381</v>
+        <v>375</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>382</v>
+        <v>376</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Course MAterials - Day 8 and 9.
</commit_message>
<xml_diff>
--- a/JEE DevOps - TOC.xlsx
+++ b/JEE DevOps - TOC.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20490" windowHeight="7815" activeTab="5"/>
+    <workbookView windowWidth="20490" windowHeight="7815" firstSheet="3" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="7" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="456" uniqueCount="377">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="465" uniqueCount="382">
   <si>
     <t>Sr. No.</t>
   </si>
@@ -675,6 +675,9 @@
     <t>Hands On Lab 2 - Spring Boot MVC Login Controller</t>
   </si>
   <si>
+    <t>spring-framework-exercises.zip</t>
+  </si>
+  <si>
     <t>Total # of Days for Spring MVC</t>
   </si>
   <si>
@@ -1074,6 +1077,9 @@
   </si>
   <si>
     <t>Hands On Lab 2 - Spring MVC with JSP</t>
+  </si>
+  <si>
+    <t>spring-data-jpa-exercises.zip</t>
   </si>
   <si>
     <t>Total # of Days for Spring  Data JPA</t>
@@ -1253,19 +1259,28 @@
     <t>Training Artifact</t>
   </si>
   <si>
+    <t>Deliverables</t>
+  </si>
+  <si>
     <t>Write correct code to pass JUnit test cases for JPA with Hibernate using PostgreSQL.</t>
   </si>
   <si>
     <t>Complete a list of exercises dedicated to  training  JPA and Hibernate ORM skills</t>
   </si>
   <si>
+    <t>Demonstrate passing test cases in IDE.</t>
+  </si>
+  <si>
     <t>Write correct code to pass JUnit test cases for various modules in Spring Core.</t>
   </si>
   <si>
     <t>Complete a list of exercises dedicated to training  Spring framework related skills.</t>
   </si>
   <si>
-    <t>spring-framework-exercises.zip</t>
+    <t>Write correct code to pass JUnit test cases for various modules in Spring Data JPA.</t>
+  </si>
+  <si>
+    <t>Complete a list of exercises dedicated to training  Spring Data JPa related skills.</t>
   </si>
 </sst>
 </file>
@@ -1273,10 +1288,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="40">
     <font>
@@ -1425,44 +1440,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1477,22 +1462,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1506,24 +1476,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1545,9 +1500,62 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1563,6 +1571,13 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1601,19 +1616,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1625,25 +1646,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1661,7 +1670,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1679,19 +1712,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1703,13 +1736,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1721,13 +1754,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1739,49 +1796,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1893,17 +1908,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1938,15 +1947,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -1958,6 +1958,21 @@
       </top>
       <bottom style="thin">
         <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1975,7 +1990,7 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="28" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1993,130 +2008,130 @@
     <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="13" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="11" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="14" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="11" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="36" fillId="22" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="32" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="33" fillId="21" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="35" fillId="21" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="13" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="39" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="38" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="37" fillId="18" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="18" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -2746,7 +2761,7 @@
   <dimension ref="A1:C55"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A36" activePane="bottomLeft" state="frozen"/>
       <selection/>
       <selection pane="bottomLeft" activeCell="C45" sqref="C45"/>
     </sheetView>
@@ -3747,12 +3762,12 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:C72"/>
+  <dimension ref="A1:C73"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A43" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A57" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="C35" sqref="C35"/>
+      <selection pane="bottomLeft" activeCell="C68" sqref="C68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" outlineLevelCol="2"/>
@@ -4240,24 +4255,31 @@
         <v>192</v>
       </c>
     </row>
-    <row r="68" ht="9" customHeight="1" spans="1:3">
-      <c r="A68" s="16"/>
-      <c r="B68" s="16"/>
-      <c r="C68" s="16"/>
-    </row>
-    <row r="71" ht="18.75" spans="1:2">
-      <c r="A71" s="23" t="s">
+    <row r="68" ht="18.75" spans="1:3">
+      <c r="A68" s="10"/>
+      <c r="B68" s="13"/>
+      <c r="C68" s="15" t="s">
         <v>193</v>
       </c>
-      <c r="B71" s="24">
-        <v>1</v>
-      </c>
+    </row>
+    <row r="69" ht="9" customHeight="1" spans="1:3">
+      <c r="A69" s="16"/>
+      <c r="B69" s="16"/>
+      <c r="C69" s="16"/>
     </row>
     <row r="72" ht="18.75" spans="1:2">
       <c r="A72" s="23" t="s">
         <v>194</v>
       </c>
       <c r="B72" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" ht="18.75" spans="1:2">
+      <c r="A73" s="23" t="s">
+        <v>195</v>
+      </c>
+      <c r="B73" s="24">
         <v>8</v>
       </c>
     </row>
@@ -4287,7 +4309,7 @@
   <dimension ref="A1:C29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
       <selection/>
       <selection pane="bottomLeft" activeCell="D7" sqref="D7"/>
     </sheetView>
@@ -4313,14 +4335,14 @@
     </row>
     <row r="2" ht="24.75" spans="1:3">
       <c r="A2" s="1" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
     </row>
     <row r="3" ht="15.75" spans="1:3">
       <c r="A3" s="7" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>20</v>
@@ -4337,10 +4359,10 @@
     <row r="5" ht="15.75" spans="1:3">
       <c r="A5" s="7"/>
       <c r="B5" s="11" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
     </row>
     <row r="6" ht="15.75" spans="1:3">
@@ -4351,24 +4373,24 @@
     <row r="7" ht="15" spans="1:3">
       <c r="A7" s="7"/>
       <c r="B7" s="11" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
     </row>
     <row r="8" ht="15" spans="1:3">
       <c r="A8" s="7"/>
       <c r="B8" s="11"/>
       <c r="C8" s="9" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
     </row>
     <row r="9" ht="15" spans="1:3">
       <c r="A9" s="7"/>
       <c r="B9" s="11"/>
       <c r="C9" s="9" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
     </row>
     <row r="10" ht="18.75" spans="1:3">
@@ -4379,7 +4401,7 @@
     <row r="11" ht="15" spans="1:3">
       <c r="A11" s="7"/>
       <c r="B11" s="11" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="C11" s="9" t="s">
         <v>74</v>
@@ -4389,14 +4411,14 @@
       <c r="A12" s="7"/>
       <c r="B12" s="11"/>
       <c r="C12" s="9" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
     </row>
     <row r="13" ht="15" spans="1:3">
       <c r="A13" s="7"/>
       <c r="B13" s="11"/>
       <c r="C13" s="9" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
     </row>
     <row r="14" ht="15.75" spans="1:3">
@@ -4407,7 +4429,7 @@
     <row r="15" ht="15" spans="1:3">
       <c r="A15" s="7"/>
       <c r="B15" s="11" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="C15" s="9" t="s">
         <v>74</v>
@@ -4417,14 +4439,14 @@
       <c r="A16" s="7"/>
       <c r="B16" s="11"/>
       <c r="C16" s="9" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
     </row>
     <row r="17" ht="15" spans="1:3">
       <c r="A17" s="7"/>
       <c r="B17" s="11"/>
       <c r="C17" s="9" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
     </row>
     <row r="18" ht="15" spans="1:3">
@@ -4435,24 +4457,24 @@
     <row r="19" ht="15" spans="1:3">
       <c r="A19" s="7"/>
       <c r="B19" s="11" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
     </row>
     <row r="20" ht="15" spans="1:3">
       <c r="A20" s="7"/>
       <c r="B20" s="11"/>
       <c r="C20" s="9" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
     </row>
     <row r="21" ht="15" spans="1:3">
       <c r="A21" s="7"/>
       <c r="B21" s="11"/>
       <c r="C21" s="9" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
     </row>
     <row r="22" ht="15" spans="1:3">
@@ -4461,14 +4483,14 @@
         <v>66</v>
       </c>
       <c r="C22" s="14" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
     </row>
     <row r="23" ht="20" customHeight="1" spans="1:3">
       <c r="A23" s="7"/>
       <c r="B23" s="13"/>
       <c r="C23" s="26" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
     </row>
     <row r="24" spans="1:3">
@@ -4483,7 +4505,7 @@
     </row>
     <row r="28" ht="18.75" spans="1:2">
       <c r="A28" s="23" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="B28" s="24">
         <v>1</v>
@@ -4491,7 +4513,7 @@
     </row>
     <row r="29" ht="18.75" spans="1:2">
       <c r="A29" s="23" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="B29" s="24">
         <v>8</v>
@@ -4516,12 +4538,12 @@
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:C126"/>
+  <dimension ref="A1:C127"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A58" activePane="bottomLeft" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A111" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="F59" sqref="F59"/>
+      <selection pane="bottomLeft" activeCell="C121" sqref="C121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" outlineLevelCol="2"/>
@@ -4544,14 +4566,14 @@
     </row>
     <row r="2" ht="24.75" spans="1:3">
       <c r="A2" s="1" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
     </row>
     <row r="3" ht="15.75" spans="1:3">
       <c r="A3" s="10" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>20</v>
@@ -4568,7 +4590,7 @@
     <row r="5" ht="15" spans="1:3">
       <c r="A5" s="10"/>
       <c r="B5" s="11" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="C5" s="9" t="s">
         <v>20</v>
@@ -4578,28 +4600,28 @@
       <c r="A6" s="10"/>
       <c r="B6" s="11"/>
       <c r="C6" s="9" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
     </row>
     <row r="7" ht="15" spans="1:3">
       <c r="A7" s="10"/>
       <c r="B7" s="11"/>
       <c r="C7" s="9" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
     </row>
     <row r="8" ht="15" spans="1:3">
       <c r="A8" s="10"/>
       <c r="B8" s="11"/>
       <c r="C8" s="9" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
     </row>
     <row r="9" ht="15" spans="1:3">
       <c r="A9" s="10"/>
       <c r="B9" s="11"/>
       <c r="C9" s="9" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
     </row>
     <row r="10" ht="15" spans="1:3">
@@ -4624,7 +4646,7 @@
     <row r="13" ht="18.75" spans="1:3">
       <c r="A13" s="10"/>
       <c r="B13" s="11" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="C13" s="19" t="s">
         <v>74</v>
@@ -4634,7 +4656,7 @@
       <c r="A14" s="10"/>
       <c r="B14" s="11"/>
       <c r="C14" s="9" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
     </row>
     <row r="15" ht="18.75" spans="1:3">
@@ -4648,35 +4670,35 @@
       <c r="A16" s="10"/>
       <c r="B16" s="11"/>
       <c r="C16" s="19" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
     </row>
     <row r="17" ht="18.75" spans="1:3">
       <c r="A17" s="10"/>
       <c r="B17" s="11"/>
       <c r="C17" s="19" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
     </row>
     <row r="18" ht="18.75" spans="1:3">
       <c r="A18" s="10"/>
       <c r="B18" s="11"/>
       <c r="C18" s="19" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
     </row>
     <row r="19" ht="18.75" spans="1:3">
       <c r="A19" s="10"/>
       <c r="B19" s="11"/>
       <c r="C19" s="19" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
     <row r="20" ht="18.75" spans="1:3">
       <c r="A20" s="10"/>
       <c r="B20" s="11"/>
       <c r="C20" s="19" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
     </row>
     <row r="21" ht="18.75" spans="1:3">
@@ -4693,7 +4715,7 @@
     <row r="23" ht="18.75" spans="1:3">
       <c r="A23" s="10"/>
       <c r="B23" s="11" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="C23" s="19" t="s">
         <v>74</v>
@@ -4710,42 +4732,42 @@
       <c r="A25" s="10"/>
       <c r="B25" s="11"/>
       <c r="C25" s="19" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
     </row>
     <row r="26" ht="18.75" spans="1:3">
       <c r="A26" s="10"/>
       <c r="B26" s="11"/>
       <c r="C26" s="19" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
     </row>
     <row r="27" ht="18.75" spans="1:3">
       <c r="A27" s="10"/>
       <c r="B27" s="11"/>
       <c r="C27" s="19" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
     </row>
     <row r="28" ht="18.75" spans="1:3">
       <c r="A28" s="10"/>
       <c r="B28" s="11"/>
       <c r="C28" s="19" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
     </row>
     <row r="29" ht="18.75" spans="1:3">
       <c r="A29" s="10"/>
       <c r="B29" s="11"/>
       <c r="C29" s="19" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
     </row>
     <row r="30" ht="18.75" spans="1:3">
       <c r="A30" s="10"/>
       <c r="B30" s="11"/>
       <c r="C30" s="19" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
     </row>
     <row r="31" ht="18.75" spans="1:3">
@@ -4763,7 +4785,7 @@
     <row r="33" ht="18.75" spans="1:3">
       <c r="A33" s="10"/>
       <c r="B33" s="11" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="C33" s="19" t="s">
         <v>74</v>
@@ -4773,77 +4795,77 @@
       <c r="A34" s="10"/>
       <c r="B34" s="11"/>
       <c r="C34" s="19" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
     </row>
     <row r="35" ht="18.75" spans="1:3">
       <c r="A35" s="10"/>
       <c r="B35" s="11"/>
       <c r="C35" s="19" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
     </row>
     <row r="36" ht="18.75" spans="1:3">
       <c r="A36" s="10"/>
       <c r="B36" s="11"/>
       <c r="C36" s="19" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
     </row>
     <row r="37" ht="18.75" spans="1:3">
       <c r="A37" s="10"/>
       <c r="B37" s="11"/>
       <c r="C37" s="19" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
     </row>
     <row r="38" ht="18.75" spans="1:3">
       <c r="A38" s="10"/>
       <c r="B38" s="11"/>
       <c r="C38" s="19" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
     </row>
     <row r="39" ht="18.75" spans="1:3">
       <c r="A39" s="10"/>
       <c r="B39" s="11"/>
       <c r="C39" s="19" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
     </row>
     <row r="40" ht="18.75" spans="1:3">
       <c r="A40" s="10"/>
       <c r="B40" s="11"/>
       <c r="C40" s="19" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
     </row>
     <row r="41" ht="18.75" spans="1:3">
       <c r="A41" s="10"/>
       <c r="B41" s="11"/>
       <c r="C41" s="19" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
     </row>
     <row r="42" ht="18.75" spans="1:3">
       <c r="A42" s="10"/>
       <c r="B42" s="11"/>
       <c r="C42" s="19" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
     </row>
     <row r="43" ht="18.75" spans="1:3">
       <c r="A43" s="10"/>
       <c r="B43" s="11"/>
       <c r="C43" s="19" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
     </row>
     <row r="44" ht="18.75" spans="1:3">
       <c r="A44" s="10"/>
       <c r="B44" s="11"/>
       <c r="C44" s="19" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
     </row>
     <row r="45" spans="1:3">
@@ -4853,7 +4875,7 @@
     <row r="46" ht="18.75" spans="1:3">
       <c r="A46" s="10"/>
       <c r="B46" s="11" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="C46" s="19" t="s">
         <v>74</v>
@@ -4863,98 +4885,98 @@
       <c r="A47" s="10"/>
       <c r="B47" s="11"/>
       <c r="C47" s="19" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
     </row>
     <row r="48" ht="18.75" spans="1:3">
       <c r="A48" s="10"/>
       <c r="B48" s="11"/>
       <c r="C48" s="19" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
     </row>
     <row r="49" ht="18.75" spans="1:3">
       <c r="A49" s="10"/>
       <c r="B49" s="11"/>
       <c r="C49" s="19" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
     </row>
     <row r="50" ht="18.75" spans="1:3">
       <c r="A50" s="10"/>
       <c r="B50" s="11"/>
       <c r="C50" s="19" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
     </row>
     <row r="51" ht="18.75" spans="1:3">
       <c r="A51" s="10"/>
       <c r="B51" s="11"/>
       <c r="C51" s="19" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
     </row>
     <row r="52" ht="18.75" spans="1:3">
       <c r="A52" s="10"/>
       <c r="B52" s="11"/>
       <c r="C52" s="19" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
     </row>
     <row r="53" ht="18.75" spans="1:3">
       <c r="A53" s="10"/>
       <c r="B53" s="11"/>
       <c r="C53" s="19" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
     </row>
     <row r="54" ht="18.75" spans="1:3">
       <c r="A54" s="10"/>
       <c r="B54" s="11"/>
       <c r="C54" s="19" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
     </row>
     <row r="55" ht="18.75" spans="1:3">
       <c r="A55" s="10"/>
       <c r="B55" s="11"/>
       <c r="C55" s="19" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
     </row>
     <row r="56" ht="18.75" spans="1:3">
       <c r="A56" s="10"/>
       <c r="B56" s="11"/>
       <c r="C56" s="19" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
     </row>
     <row r="57" ht="18.75" spans="1:3">
       <c r="A57" s="10"/>
       <c r="B57" s="11"/>
       <c r="C57" s="19" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
     </row>
     <row r="58" ht="18.75" spans="1:3">
       <c r="A58" s="10"/>
       <c r="B58" s="11"/>
       <c r="C58" s="19" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
     </row>
     <row r="59" ht="18.75" spans="1:3">
       <c r="A59" s="10"/>
       <c r="B59" s="11"/>
       <c r="C59" s="19" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
     </row>
     <row r="60" ht="18.75" spans="1:3">
       <c r="A60" s="10"/>
       <c r="B60" s="11"/>
       <c r="C60" s="19" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
     </row>
     <row r="61" spans="1:3">
@@ -4964,7 +4986,7 @@
     <row r="62" ht="18.75" spans="1:3">
       <c r="A62" s="10"/>
       <c r="B62" s="11" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="C62" s="19" t="s">
         <v>74</v>
@@ -4974,42 +4996,42 @@
       <c r="A63" s="10"/>
       <c r="B63" s="11"/>
       <c r="C63" s="19" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
     </row>
     <row r="64" ht="18.75" spans="1:3">
       <c r="A64" s="10"/>
       <c r="B64" s="11"/>
       <c r="C64" s="19" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
     <row r="65" ht="18.75" spans="1:3">
       <c r="A65" s="10"/>
       <c r="B65" s="11"/>
       <c r="C65" s="19" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="66" ht="18.75" spans="1:3">
       <c r="A66" s="10"/>
       <c r="B66" s="11"/>
       <c r="C66" s="19" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
     </row>
     <row r="67" ht="18.75" spans="1:3">
       <c r="A67" s="10"/>
       <c r="B67" s="11"/>
       <c r="C67" s="19" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
     </row>
     <row r="68" ht="18.75" spans="1:3">
       <c r="A68" s="10"/>
       <c r="B68" s="11"/>
       <c r="C68" s="19" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
     </row>
     <row r="69" ht="18.75" spans="1:3">
@@ -5026,7 +5048,7 @@
     <row r="71" ht="18.75" spans="1:3">
       <c r="A71" s="10"/>
       <c r="B71" s="11" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="C71" s="19" t="s">
         <v>74</v>
@@ -5036,112 +5058,112 @@
       <c r="A72" s="10"/>
       <c r="B72" s="11"/>
       <c r="C72" s="19" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
     </row>
     <row r="73" ht="18.75" spans="1:3">
       <c r="A73" s="10"/>
       <c r="B73" s="11"/>
       <c r="C73" s="19" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
     </row>
     <row r="74" ht="18.75" spans="1:3">
       <c r="A74" s="10"/>
       <c r="B74" s="11"/>
       <c r="C74" s="19" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
     </row>
     <row r="75" ht="18.75" spans="1:3">
       <c r="A75" s="10"/>
       <c r="B75" s="11"/>
       <c r="C75" s="19" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row r="76" ht="18.75" spans="1:3">
       <c r="A76" s="10"/>
       <c r="B76" s="11"/>
       <c r="C76" s="19" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
     </row>
     <row r="77" ht="18.75" spans="1:3">
       <c r="A77" s="10"/>
       <c r="B77" s="11"/>
       <c r="C77" s="19" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
     </row>
     <row r="78" ht="18.75" spans="1:3">
       <c r="A78" s="10"/>
       <c r="B78" s="11"/>
       <c r="C78" s="19" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
     </row>
     <row r="79" ht="18.75" spans="1:3">
       <c r="A79" s="10"/>
       <c r="B79" s="11"/>
       <c r="C79" s="19" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
     </row>
     <row r="80" ht="18.75" spans="1:3">
       <c r="A80" s="10"/>
       <c r="B80" s="11"/>
       <c r="C80" s="19" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
     </row>
     <row r="81" ht="18.75" spans="1:3">
       <c r="A81" s="10"/>
       <c r="B81" s="11"/>
       <c r="C81" s="19" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
     </row>
     <row r="82" ht="18.75" spans="1:3">
       <c r="A82" s="10"/>
       <c r="B82" s="11"/>
       <c r="C82" s="19" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
     </row>
     <row r="83" ht="18.75" spans="1:3">
       <c r="A83" s="10"/>
       <c r="B83" s="11"/>
       <c r="C83" s="19" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
     </row>
     <row r="84" ht="18.75" spans="1:3">
       <c r="A84" s="10"/>
       <c r="B84" s="11"/>
       <c r="C84" s="19" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
     </row>
     <row r="85" ht="18.75" spans="1:3">
       <c r="A85" s="10"/>
       <c r="B85" s="11"/>
       <c r="C85" s="19" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
     </row>
     <row r="86" ht="18.75" spans="1:3">
       <c r="A86" s="10"/>
       <c r="B86" s="11"/>
       <c r="C86" s="19" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
     </row>
     <row r="87" ht="18.75" spans="1:3">
       <c r="A87" s="10"/>
       <c r="B87" s="11"/>
       <c r="C87" s="19" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
     </row>
     <row r="88" ht="18.75" spans="1:3">
@@ -5155,21 +5177,21 @@
         <v>66</v>
       </c>
       <c r="C89" s="20" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
     </row>
     <row r="90" ht="18.75" spans="1:3">
       <c r="A90" s="10"/>
       <c r="B90" s="13"/>
       <c r="C90" s="19" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
     </row>
     <row r="91" ht="18.75" spans="1:3">
       <c r="A91" s="10"/>
       <c r="B91" s="13"/>
       <c r="C91" s="19" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
     </row>
     <row r="92" spans="1:3">
@@ -5179,69 +5201,69 @@
     </row>
     <row r="93" ht="24.75" spans="1:3">
       <c r="A93" s="1" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="B93" s="1"/>
       <c r="C93" s="1"/>
     </row>
     <row r="94" ht="18.75" spans="1:3">
       <c r="A94" s="10" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="B94" s="21" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="C94" s="19" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
     </row>
     <row r="95" ht="18.75" spans="1:3">
       <c r="A95" s="10"/>
       <c r="B95" s="21"/>
       <c r="C95" s="19" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
     </row>
     <row r="96" ht="18.75" spans="1:3">
       <c r="A96" s="10"/>
       <c r="B96" s="21"/>
       <c r="C96" s="19" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
     </row>
     <row r="97" ht="18.75" spans="1:3">
       <c r="A97" s="10"/>
       <c r="B97" s="21"/>
       <c r="C97" s="19" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
     </row>
     <row r="98" ht="18.75" spans="1:3">
       <c r="A98" s="10"/>
       <c r="B98" s="21"/>
       <c r="C98" s="19" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
     </row>
     <row r="99" ht="18.75" spans="1:3">
       <c r="A99" s="10"/>
       <c r="B99" s="21"/>
       <c r="C99" s="19" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
     </row>
     <row r="100" ht="18.75" spans="1:3">
       <c r="A100" s="10"/>
       <c r="B100" s="21"/>
       <c r="C100" s="19" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
     </row>
     <row r="101" ht="18.75" spans="1:3">
       <c r="A101" s="10"/>
       <c r="B101" s="21"/>
       <c r="C101" s="19" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
     </row>
     <row r="102" spans="1:3">
@@ -5251,7 +5273,7 @@
     <row r="103" ht="18.75" spans="1:3">
       <c r="A103" s="10"/>
       <c r="B103" s="21" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="C103" s="19" t="s">
         <v>74</v>
@@ -5261,98 +5283,98 @@
       <c r="A104" s="10"/>
       <c r="B104" s="21"/>
       <c r="C104" s="19" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
     </row>
     <row r="105" ht="18.75" spans="1:3">
       <c r="A105" s="10"/>
       <c r="B105" s="21"/>
       <c r="C105" s="19" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
     </row>
     <row r="106" ht="18.75" spans="1:3">
       <c r="A106" s="10"/>
       <c r="B106" s="21"/>
       <c r="C106" s="19" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
     </row>
     <row r="107" ht="18.75" spans="1:3">
       <c r="A107" s="10"/>
       <c r="B107" s="21"/>
       <c r="C107" s="19" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
     </row>
     <row r="108" ht="18.75" spans="1:3">
       <c r="A108" s="10"/>
       <c r="B108" s="21"/>
       <c r="C108" s="19" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
     </row>
     <row r="109" ht="18.75" spans="1:3">
       <c r="A109" s="10"/>
       <c r="B109" s="21"/>
       <c r="C109" s="19" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
     </row>
     <row r="110" ht="18.75" spans="1:3">
       <c r="A110" s="10"/>
       <c r="B110" s="21"/>
       <c r="C110" s="19" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
     </row>
     <row r="111" ht="18.75" spans="1:3">
       <c r="A111" s="10"/>
       <c r="B111" s="21"/>
       <c r="C111" s="19" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
     </row>
     <row r="112" ht="18.75" spans="1:3">
       <c r="A112" s="10"/>
       <c r="B112" s="21"/>
       <c r="C112" s="19" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
     </row>
     <row r="113" ht="18.75" spans="1:3">
       <c r="A113" s="10"/>
       <c r="B113" s="21"/>
       <c r="C113" s="19" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
     </row>
     <row r="114" ht="37.5" spans="1:3">
       <c r="A114" s="10"/>
       <c r="B114" s="21"/>
       <c r="C114" s="19" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
     </row>
     <row r="115" ht="18.75" spans="1:3">
       <c r="A115" s="10"/>
       <c r="B115" s="21"/>
       <c r="C115" s="19" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
     </row>
     <row r="116" ht="18.75" spans="1:3">
       <c r="A116" s="10"/>
       <c r="B116" s="21"/>
       <c r="C116" s="19" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
     </row>
     <row r="117" ht="18.75" spans="1:3">
       <c r="A117" s="10"/>
       <c r="B117" s="21"/>
       <c r="C117" s="19" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
     </row>
     <row r="118" spans="1:3">
@@ -5363,37 +5385,44 @@
     <row r="119" ht="37.5" spans="1:3">
       <c r="A119" s="10"/>
       <c r="B119" s="22" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="C119" s="19" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
     </row>
     <row r="120" ht="18.75" spans="1:3">
       <c r="A120" s="10"/>
       <c r="B120" s="22"/>
       <c r="C120" s="19" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="121" spans="1:3">
-      <c r="A121" s="16"/>
-      <c r="B121" s="16"/>
-      <c r="C121" s="16"/>
-    </row>
-    <row r="125" ht="18.75" spans="1:2">
-      <c r="A125" s="23" t="s">
         <v>320</v>
       </c>
-      <c r="B125" s="24">
-        <v>2</v>
-      </c>
+    </row>
+    <row r="121" ht="18.75" spans="1:3">
+      <c r="A121" s="10"/>
+      <c r="B121" s="22"/>
+      <c r="C121" s="19" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3">
+      <c r="A122" s="16"/>
+      <c r="B122" s="16"/>
+      <c r="C122" s="16"/>
     </row>
     <row r="126" ht="18.75" spans="1:2">
       <c r="A126" s="23" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="B126" s="24">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="127" ht="18.75" spans="1:2">
+      <c r="A127" s="23" t="s">
+        <v>323</v>
+      </c>
+      <c r="B127" s="24">
         <v>16</v>
       </c>
     </row>
@@ -5452,14 +5481,14 @@
     </row>
     <row r="2" ht="24.75" spans="1:3">
       <c r="A2" s="1" t="s">
-        <v>322</v>
+        <v>324</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
     </row>
     <row r="3" ht="15.75" spans="1:3">
       <c r="A3" s="7" t="s">
-        <v>323</v>
+        <v>325</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>20</v>
@@ -5476,7 +5505,7 @@
     <row r="5" ht="15" spans="1:3">
       <c r="A5" s="10"/>
       <c r="B5" s="11" t="s">
-        <v>324</v>
+        <v>326</v>
       </c>
       <c r="C5" s="9" t="s">
         <v>74</v>
@@ -5486,70 +5515,70 @@
       <c r="A6" s="10"/>
       <c r="B6" s="11"/>
       <c r="C6" s="9" t="s">
-        <v>325</v>
+        <v>327</v>
       </c>
     </row>
     <row r="7" ht="15" spans="1:3">
       <c r="A7" s="10"/>
       <c r="B7" s="11"/>
       <c r="C7" s="9" t="s">
-        <v>326</v>
+        <v>328</v>
       </c>
     </row>
     <row r="8" ht="15" spans="1:3">
       <c r="A8" s="10"/>
       <c r="B8" s="11"/>
       <c r="C8" s="9" t="s">
-        <v>327</v>
+        <v>329</v>
       </c>
     </row>
     <row r="9" ht="15" spans="1:3">
       <c r="A9" s="10"/>
       <c r="B9" s="11"/>
       <c r="C9" s="9" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
     </row>
     <row r="10" ht="15" spans="1:3">
       <c r="A10" s="10"/>
       <c r="B10" s="11"/>
       <c r="C10" s="9" t="s">
-        <v>329</v>
+        <v>331</v>
       </c>
     </row>
     <row r="11" ht="15" spans="1:3">
       <c r="A11" s="10"/>
       <c r="B11" s="11"/>
       <c r="C11" s="9" t="s">
-        <v>330</v>
+        <v>332</v>
       </c>
     </row>
     <row r="12" ht="15" spans="1:3">
       <c r="A12" s="10"/>
       <c r="B12" s="11"/>
       <c r="C12" s="9" t="s">
-        <v>331</v>
+        <v>333</v>
       </c>
     </row>
     <row r="13" ht="15" spans="1:3">
       <c r="A13" s="10"/>
       <c r="B13" s="11"/>
       <c r="C13" s="9" t="s">
-        <v>332</v>
+        <v>334</v>
       </c>
     </row>
     <row r="14" ht="15" spans="1:3">
       <c r="A14" s="10"/>
       <c r="B14" s="11"/>
       <c r="C14" s="9" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
     </row>
     <row r="15" ht="15" spans="1:3">
       <c r="A15" s="10"/>
       <c r="B15" s="11"/>
       <c r="C15" s="9" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
     </row>
     <row r="16" ht="15.75" spans="1:3">
@@ -5560,7 +5589,7 @@
     <row r="17" ht="15" spans="1:3">
       <c r="A17" s="10"/>
       <c r="B17" s="11" t="s">
-        <v>335</v>
+        <v>337</v>
       </c>
       <c r="C17" s="9" t="s">
         <v>74</v>
@@ -5570,49 +5599,49 @@
       <c r="A18" s="10"/>
       <c r="B18" s="11"/>
       <c r="C18" s="9" t="s">
-        <v>336</v>
+        <v>338</v>
       </c>
     </row>
     <row r="19" ht="15" spans="1:3">
       <c r="A19" s="10"/>
       <c r="B19" s="11"/>
       <c r="C19" s="9" t="s">
-        <v>337</v>
+        <v>339</v>
       </c>
     </row>
     <row r="20" ht="15" spans="1:3">
       <c r="A20" s="10"/>
       <c r="B20" s="11"/>
       <c r="C20" s="9" t="s">
-        <v>338</v>
+        <v>340</v>
       </c>
     </row>
     <row r="21" ht="15" spans="1:3">
       <c r="A21" s="10"/>
       <c r="B21" s="11"/>
       <c r="C21" s="9" t="s">
-        <v>339</v>
+        <v>341</v>
       </c>
     </row>
     <row r="22" ht="15" spans="1:3">
       <c r="A22" s="10"/>
       <c r="B22" s="11"/>
       <c r="C22" s="9" t="s">
-        <v>340</v>
+        <v>342</v>
       </c>
     </row>
     <row r="23" ht="15" spans="1:3">
       <c r="A23" s="10"/>
       <c r="B23" s="11"/>
       <c r="C23" s="9" t="s">
-        <v>341</v>
+        <v>343</v>
       </c>
     </row>
     <row r="24" ht="15" spans="1:3">
       <c r="A24" s="10"/>
       <c r="B24" s="11"/>
       <c r="C24" s="9" t="s">
-        <v>342</v>
+        <v>344</v>
       </c>
     </row>
     <row r="25" ht="15" spans="1:3">
@@ -5633,14 +5662,14 @@
         <v>66</v>
       </c>
       <c r="C27" s="14" t="s">
-        <v>343</v>
+        <v>345</v>
       </c>
     </row>
     <row r="28" ht="20" customHeight="1" spans="1:3">
       <c r="A28" s="10"/>
       <c r="B28" s="13"/>
       <c r="C28" s="15" t="s">
-        <v>344</v>
+        <v>346</v>
       </c>
     </row>
     <row r="29" ht="8" customHeight="1" spans="1:3">
@@ -5650,17 +5679,17 @@
     </row>
     <row r="30" customFormat="1" ht="24.75" spans="1:3">
       <c r="A30" s="1" t="s">
-        <v>345</v>
+        <v>347</v>
       </c>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
     </row>
     <row r="31" ht="15" spans="1:3">
       <c r="A31" s="17" t="s">
-        <v>346</v>
+        <v>348</v>
       </c>
       <c r="B31" s="11" t="s">
-        <v>347</v>
+        <v>349</v>
       </c>
       <c r="C31" s="9" t="s">
         <v>74</v>
@@ -5670,56 +5699,56 @@
       <c r="A32" s="17"/>
       <c r="B32" s="11"/>
       <c r="C32" s="9" t="s">
-        <v>348</v>
+        <v>350</v>
       </c>
     </row>
     <row r="33" ht="15" spans="1:3">
       <c r="A33" s="17"/>
       <c r="B33" s="11"/>
       <c r="C33" s="9" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
     </row>
     <row r="34" ht="15" spans="1:3">
       <c r="A34" s="17"/>
       <c r="B34" s="11"/>
       <c r="C34" s="9" t="s">
-        <v>350</v>
+        <v>352</v>
       </c>
     </row>
     <row r="35" ht="15" spans="1:3">
       <c r="A35" s="17"/>
       <c r="B35" s="11"/>
       <c r="C35" s="9" t="s">
-        <v>351</v>
+        <v>353</v>
       </c>
     </row>
     <row r="36" ht="15" spans="1:3">
       <c r="A36" s="17"/>
       <c r="B36" s="11"/>
       <c r="C36" s="9" t="s">
-        <v>352</v>
+        <v>354</v>
       </c>
     </row>
     <row r="37" ht="15" spans="1:3">
       <c r="A37" s="17"/>
       <c r="B37" s="11"/>
       <c r="C37" s="9" t="s">
-        <v>353</v>
+        <v>355</v>
       </c>
     </row>
     <row r="38" ht="15" spans="1:3">
       <c r="A38" s="17"/>
       <c r="B38" s="11"/>
       <c r="C38" s="9" t="s">
-        <v>354</v>
+        <v>356</v>
       </c>
     </row>
     <row r="39" ht="15" spans="1:3">
       <c r="A39" s="17"/>
       <c r="B39" s="11"/>
       <c r="C39" s="9" t="s">
-        <v>355</v>
+        <v>357</v>
       </c>
     </row>
     <row r="40" ht="15" spans="1:3">
@@ -5737,7 +5766,7 @@
     <row r="42" ht="15" spans="1:3">
       <c r="A42" s="17"/>
       <c r="B42" s="11" t="s">
-        <v>356</v>
+        <v>358</v>
       </c>
       <c r="C42" s="9" t="s">
         <v>74</v>
@@ -5747,77 +5776,77 @@
       <c r="A43" s="17"/>
       <c r="B43" s="11"/>
       <c r="C43" s="9" t="s">
-        <v>357</v>
+        <v>359</v>
       </c>
     </row>
     <row r="44" ht="15" spans="1:3">
       <c r="A44" s="17"/>
       <c r="B44" s="11"/>
       <c r="C44" s="9" t="s">
-        <v>358</v>
+        <v>360</v>
       </c>
     </row>
     <row r="45" ht="15" spans="1:3">
       <c r="A45" s="17"/>
       <c r="B45" s="11"/>
       <c r="C45" s="9" t="s">
-        <v>359</v>
+        <v>361</v>
       </c>
     </row>
     <row r="46" ht="15" spans="1:3">
       <c r="A46" s="17"/>
       <c r="B46" s="11"/>
       <c r="C46" s="9" t="s">
-        <v>360</v>
+        <v>362</v>
       </c>
     </row>
     <row r="47" ht="15" spans="1:3">
       <c r="A47" s="17"/>
       <c r="B47" s="11"/>
       <c r="C47" s="9" t="s">
-        <v>361</v>
+        <v>363</v>
       </c>
     </row>
     <row r="48" ht="15" spans="1:3">
       <c r="A48" s="17"/>
       <c r="B48" s="11"/>
       <c r="C48" s="9" t="s">
-        <v>362</v>
+        <v>364</v>
       </c>
     </row>
     <row r="49" ht="15" spans="1:3">
       <c r="A49" s="17"/>
       <c r="B49" s="11"/>
       <c r="C49" s="9" t="s">
-        <v>363</v>
+        <v>365</v>
       </c>
     </row>
     <row r="50" ht="15" spans="1:3">
       <c r="A50" s="17"/>
       <c r="B50" s="11"/>
       <c r="C50" s="9" t="s">
-        <v>364</v>
+        <v>366</v>
       </c>
     </row>
     <row r="51" spans="1:3">
       <c r="A51" s="17"/>
       <c r="B51" s="11"/>
       <c r="C51" s="12" t="s">
-        <v>365</v>
+        <v>367</v>
       </c>
     </row>
     <row r="52" spans="1:3">
       <c r="A52" s="17"/>
       <c r="B52" s="11"/>
       <c r="C52" s="12" t="s">
-        <v>366</v>
+        <v>368</v>
       </c>
     </row>
     <row r="53" spans="1:3">
       <c r="A53" s="17"/>
       <c r="B53" s="11"/>
       <c r="C53" s="12" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
     </row>
     <row r="54" ht="15" spans="1:3">
@@ -5826,14 +5855,14 @@
         <v>66</v>
       </c>
       <c r="C54" s="14" t="s">
-        <v>343</v>
+        <v>345</v>
       </c>
     </row>
     <row r="55" ht="15" spans="1:3">
       <c r="A55" s="17"/>
       <c r="B55" s="13"/>
       <c r="C55" s="15" t="s">
-        <v>367</v>
+        <v>369</v>
       </c>
     </row>
     <row r="56" customFormat="1" ht="9" customHeight="1" spans="1:3">
@@ -5943,15 +5972,15 @@
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="C15" sqref="C15"/>
+      <selection pane="bottomLeft" activeCell="E1" sqref="E$1:E$1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" outlineLevelRow="5" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" outlineLevelRow="7" outlineLevelCol="4"/>
   <cols>
     <col min="1" max="1" width="23.875" customWidth="1"/>
     <col min="2" max="2" width="38.25" customWidth="1"/>
@@ -5962,52 +5991,78 @@
   <sheetData>
     <row r="1" customFormat="1" ht="24.75" spans="1:4">
       <c r="A1" s="1" t="s">
-        <v>345</v>
+        <v>347</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
     </row>
-    <row r="2" ht="15" spans="1:4">
+    <row r="2" ht="15" spans="1:5">
       <c r="A2" s="2" t="s">
-        <v>368</v>
+        <v>370</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>369</v>
+        <v>371</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>370</v>
+        <v>372</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>371</v>
-      </c>
-    </row>
-    <row r="4" ht="25.5" spans="1:4">
+        <v>373</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="4" ht="25.5" spans="1:5">
       <c r="A4" s="3">
         <v>1</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>372</v>
+        <v>375</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>373</v>
+        <v>376</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="6" ht="25.5" spans="1:4">
+      <c r="E4" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="6" ht="25.5" spans="1:5">
       <c r="A6" s="3">
         <v>2</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>374</v>
+        <v>378</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>375</v>
+        <v>379</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>376</v>
+        <v>193</v>
+      </c>
+      <c r="E6" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="8" ht="25.5" spans="1:5">
+      <c r="A8" s="3">
+        <v>3</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>380</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>381</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>321</v>
+      </c>
+      <c r="E8" t="s">
+        <v>377</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Course MAterials - Day 10 - Swagger.
</commit_message>
<xml_diff>
--- a/JEE DevOps - TOC.xlsx
+++ b/JEE DevOps - TOC.xlsx
@@ -14,14 +14,15 @@
     <sheet name="Spring REST" sheetId="15" r:id="rId5"/>
     <sheet name="Spring  Data JPA" sheetId="16" r:id="rId6"/>
     <sheet name="Spring Data REST" sheetId="17" r:id="rId7"/>
-    <sheet name="Sprint 1 Evaluation" sheetId="18" r:id="rId8"/>
+    <sheet name="Swagger" sheetId="19" r:id="rId8"/>
+    <sheet name="Sprint 1 Evaluation" sheetId="18" r:id="rId9"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="465" uniqueCount="382">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="504" uniqueCount="413">
   <si>
     <t>Sr. No.</t>
   </si>
@@ -1247,6 +1248,119 @@
     <t>Hands On Lab 2 - Expose RESTful APIs around Spring Data Repositories</t>
   </si>
   <si>
+    <t>Day 10</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color rgb="FF00B0F0"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Swagger Tools is the leading platform for describing RESTful web services.                                      </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Learn how to use Swagger Tools to describe, document, generate code, and test RESTful web APIs based on the OpenAPI standard.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">2. Introduction </t>
+  </si>
+  <si>
+    <t>2. The Swagger Tools</t>
+  </si>
+  <si>
+    <t>3. Setup Free Swagger Account</t>
+  </si>
+  <si>
+    <t>4. The Demo Code</t>
+  </si>
+  <si>
+    <t>3. Create OpenAPI Documents with Swagger Editor</t>
+  </si>
+  <si>
+    <t>1. Navigating the Swagger Editor</t>
+  </si>
+  <si>
+    <t>2. OpenAPI 2.0: Version and Info</t>
+  </si>
+  <si>
+    <t>3. OpenAPI 2.0: Paths and GET Operation</t>
+  </si>
+  <si>
+    <t>4. OpenAPI 2.0: Produces, Consumes and Parameters</t>
+  </si>
+  <si>
+    <t>5. OpenAPI 2.0: Responses</t>
+  </si>
+  <si>
+    <t>6. OpenAPI 2.0: References and Definitions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7. OpenAPI 2.0: Post, Put, Delete </t>
+  </si>
+  <si>
+    <t>8. OpenAPI 2.0: Host, Schema, and BasePath</t>
+  </si>
+  <si>
+    <t>9. OpenAPI 2.0: SecurityDefinitions and Security</t>
+  </si>
+  <si>
+    <t>Swagger Editor</t>
+  </si>
+  <si>
+    <t>Hands On Lab 1- Create Your First OpenAPI Definition with Swagger Editor</t>
+  </si>
+  <si>
+    <t>Day 11</t>
+  </si>
+  <si>
+    <t>Explore the Swagger Editor, Swagger UI, and Swagger Inspector to describe, document, and test RESTful web APIs.                                             Discover how to auto-generate code in several languages from OpenAPI documents.</t>
+  </si>
+  <si>
+    <t>4. OpenAPI 2.0 vs. OpenAPI 3.0</t>
+  </si>
+  <si>
+    <t>1. Converting to OpenAPI 3.0</t>
+  </si>
+  <si>
+    <t>2. The Content and RequestBody Fields</t>
+  </si>
+  <si>
+    <t>3. Servers, Security and Component</t>
+  </si>
+  <si>
+    <t>5. Document OpenAPI with Swagger UI</t>
+  </si>
+  <si>
+    <t>1. URL, Security, Operations, and Parameters</t>
+  </si>
+  <si>
+    <t>2. Operations, Model, Example Values, and Responses</t>
+  </si>
+  <si>
+    <t>6. Interacting with Web APIs Using Swagger Inspector and Codegen</t>
+  </si>
+  <si>
+    <t>1. Testing a Web API</t>
+  </si>
+  <si>
+    <t>2. Interrogating a Web API</t>
+  </si>
+  <si>
+    <t>3. Generate Client SDKs and Server Stubs</t>
+  </si>
+  <si>
     <t>Serial Number</t>
   </si>
   <si>
@@ -1290,8 +1404,8 @@
   <numFmts count="4">
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="40">
     <font>
@@ -1453,26 +1567,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <i/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1484,11 +1583,27 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
+      <u/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1508,7 +1623,15 @@
     </font>
     <font>
       <b/>
-      <sz val="13"/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -1517,32 +1640,9 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1561,16 +1661,30 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1616,7 +1730,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1628,25 +1772,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1658,7 +1796,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1670,37 +1838,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1718,7 +1862,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1730,49 +1886,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1784,19 +1910,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1890,33 +2004,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -1928,6 +2015,15 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1962,6 +2058,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -1979,6 +2084,15 @@
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -1990,7 +2104,7 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="22" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -2008,130 +2122,130 @@
     <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="20" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="23" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="13" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="11" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="36" fillId="22" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="34" fillId="27" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="26" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="26" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="21" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="21" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="22" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -2599,7 +2713,7 @@
   <dimension ref="A7:I22"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="K20" sqref="K20"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75"/>
@@ -5455,7 +5569,7 @@
   <dimension ref="A1:C83"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A63" activePane="bottomLeft" state="frozen"/>
       <selection/>
       <selection pane="bottomLeft" activeCell="A30" sqref="$A30:$XFD30"/>
     </sheetView>
@@ -5972,10 +6086,392 @@
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
+  <dimension ref="A1:C64"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
+      <selection/>
+      <selection pane="bottomLeft" activeCell="D35" sqref="D35"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" outlineLevelCol="2"/>
+  <cols>
+    <col min="1" max="1" width="31.5" customWidth="1"/>
+    <col min="2" max="2" width="35.125" customWidth="1"/>
+    <col min="3" max="3" width="58.625" customWidth="1"/>
+    <col min="4" max="4" width="23" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="16.5" spans="1:3">
+      <c r="A1" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" ht="24.75" spans="1:3">
+      <c r="A2" s="1" t="s">
+        <v>370</v>
+      </c>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+    </row>
+    <row r="3" ht="15.75" spans="1:3">
+      <c r="A3" s="7" t="s">
+        <v>371</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" ht="15.75" spans="1:3">
+      <c r="A4" s="10"/>
+      <c r="B4" s="8"/>
+      <c r="C4" s="9"/>
+    </row>
+    <row r="5" ht="15" spans="1:3">
+      <c r="A5" s="10"/>
+      <c r="B5" s="11" t="s">
+        <v>372</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="6" ht="15" spans="1:3">
+      <c r="A6" s="10"/>
+      <c r="B6" s="11"/>
+      <c r="C6" s="9" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="7" ht="15" spans="1:3">
+      <c r="A7" s="10"/>
+      <c r="B7" s="11"/>
+      <c r="C7" s="9" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="8" ht="15" spans="1:3">
+      <c r="A8" s="10"/>
+      <c r="B8" s="11"/>
+      <c r="C8" s="9" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="9" ht="15.75" spans="1:3">
+      <c r="A9" s="10"/>
+      <c r="B9" s="11"/>
+      <c r="C9" s="9"/>
+    </row>
+    <row r="10" ht="15" spans="1:3">
+      <c r="A10" s="10"/>
+      <c r="B10" s="11" t="s">
+        <v>376</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="11" ht="15" spans="1:3">
+      <c r="A11" s="10"/>
+      <c r="B11" s="11"/>
+      <c r="C11" s="9" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="12" ht="15" spans="1:3">
+      <c r="A12" s="10"/>
+      <c r="B12" s="11"/>
+      <c r="C12" s="9" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="13" ht="15" spans="1:3">
+      <c r="A13" s="10"/>
+      <c r="B13" s="11"/>
+      <c r="C13" s="9" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="14" ht="15" spans="1:3">
+      <c r="A14" s="10"/>
+      <c r="B14" s="11"/>
+      <c r="C14" s="9" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="15" ht="15" spans="1:3">
+      <c r="A15" s="10"/>
+      <c r="B15" s="11"/>
+      <c r="C15" s="9" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="16" ht="15" spans="1:3">
+      <c r="A16" s="10"/>
+      <c r="B16" s="11"/>
+      <c r="C16" s="9" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="17" ht="15" spans="1:3">
+      <c r="A17" s="10"/>
+      <c r="B17" s="11"/>
+      <c r="C17" s="9" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="18" ht="15" spans="1:3">
+      <c r="A18" s="10"/>
+      <c r="B18" s="11"/>
+      <c r="C18" s="9" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" s="10"/>
+      <c r="B19" s="11"/>
+      <c r="C19" s="12"/>
+    </row>
+    <row r="20" ht="15" spans="1:3">
+      <c r="A20" s="10"/>
+      <c r="B20" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="C20" s="14" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="21" ht="17" customHeight="1" spans="1:3">
+      <c r="A21" s="10"/>
+      <c r="B21" s="13"/>
+      <c r="C21" s="15" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="22" ht="8" customHeight="1" spans="1:3">
+      <c r="A22" s="16"/>
+      <c r="B22" s="16"/>
+      <c r="C22" s="16"/>
+    </row>
+    <row r="23" customFormat="1" ht="24.75" spans="1:3">
+      <c r="A23" s="1" t="s">
+        <v>388</v>
+      </c>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+    </row>
+    <row r="24" ht="15" spans="1:3">
+      <c r="A24" s="17" t="s">
+        <v>389</v>
+      </c>
+      <c r="B24" s="11" t="s">
+        <v>390</v>
+      </c>
+      <c r="C24" s="9" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="25" ht="15" spans="1:3">
+      <c r="A25" s="17"/>
+      <c r="B25" s="11"/>
+      <c r="C25" s="9" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="26" ht="15" spans="1:3">
+      <c r="A26" s="17"/>
+      <c r="B26" s="11"/>
+      <c r="C26" s="9" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="27" ht="15.75" spans="1:3">
+      <c r="A27" s="17"/>
+      <c r="B27" s="18"/>
+      <c r="C27" s="9"/>
+    </row>
+    <row r="28" ht="15" spans="1:3">
+      <c r="A28" s="17"/>
+      <c r="B28" s="11" t="s">
+        <v>394</v>
+      </c>
+      <c r="C28" s="9" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="29" ht="15" spans="1:3">
+      <c r="A29" s="17"/>
+      <c r="B29" s="11"/>
+      <c r="C29" s="9" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="30" ht="15.75" spans="1:3">
+      <c r="A30" s="17"/>
+      <c r="B30" s="11"/>
+      <c r="C30" s="12"/>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31" s="17"/>
+      <c r="B31" s="11" t="s">
+        <v>397</v>
+      </c>
+      <c r="C31" s="12" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
+      <c r="A32" s="17"/>
+      <c r="B32" s="11"/>
+      <c r="C32" s="12" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33" s="17"/>
+      <c r="B33" s="11"/>
+      <c r="C33" s="12" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="34" ht="15.75" spans="1:3">
+      <c r="A34" s="17"/>
+      <c r="B34" s="11"/>
+      <c r="C34" s="12"/>
+    </row>
+    <row r="35" ht="15" spans="1:3">
+      <c r="A35" s="17"/>
+      <c r="B35" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="C35" s="14"/>
+    </row>
+    <row r="36" ht="15" spans="1:3">
+      <c r="A36" s="17"/>
+      <c r="B36" s="13"/>
+      <c r="C36" s="15"/>
+    </row>
+    <row r="37" customFormat="1" ht="9" customHeight="1" spans="1:3">
+      <c r="A37" s="16"/>
+      <c r="B37" s="16"/>
+      <c r="C37" s="16"/>
+    </row>
+    <row r="38" ht="18.75" spans="1:1">
+      <c r="A38" s="7"/>
+    </row>
+    <row r="39" ht="18.75" spans="1:1">
+      <c r="A39" s="7"/>
+    </row>
+    <row r="40" ht="18.75" spans="1:1">
+      <c r="A40" s="7"/>
+    </row>
+    <row r="41" ht="18.75" spans="1:1">
+      <c r="A41" s="7"/>
+    </row>
+    <row r="42" ht="18.75" spans="1:1">
+      <c r="A42" s="7"/>
+    </row>
+    <row r="43" ht="18.75" spans="1:1">
+      <c r="A43" s="7"/>
+    </row>
+    <row r="44" ht="18.75" spans="1:1">
+      <c r="A44" s="7"/>
+    </row>
+    <row r="45" ht="18.75" spans="1:1">
+      <c r="A45" s="7"/>
+    </row>
+    <row r="46" ht="18.75" spans="1:1">
+      <c r="A46" s="7"/>
+    </row>
+    <row r="47" ht="18.75" spans="1:1">
+      <c r="A47" s="7"/>
+    </row>
+    <row r="48" ht="18.75" spans="1:1">
+      <c r="A48" s="7"/>
+    </row>
+    <row r="49" ht="18.75" spans="1:1">
+      <c r="A49" s="7"/>
+    </row>
+    <row r="50" ht="18.75" spans="1:1">
+      <c r="A50" s="7"/>
+    </row>
+    <row r="51" ht="18.75" spans="1:1">
+      <c r="A51" s="7"/>
+    </row>
+    <row r="52" ht="18.75" spans="1:1">
+      <c r="A52" s="7"/>
+    </row>
+    <row r="53" ht="18.75" spans="1:1">
+      <c r="A53" s="7"/>
+    </row>
+    <row r="54" ht="18.75" spans="1:1">
+      <c r="A54" s="7"/>
+    </row>
+    <row r="55" ht="18.75" spans="1:1">
+      <c r="A55" s="7"/>
+    </row>
+    <row r="56" ht="18.75" spans="1:1">
+      <c r="A56" s="7"/>
+    </row>
+    <row r="57" ht="18.75" spans="1:1">
+      <c r="A57" s="7"/>
+    </row>
+    <row r="58" ht="18.75" spans="1:1">
+      <c r="A58" s="7"/>
+    </row>
+    <row r="59" ht="18.75" spans="1:1">
+      <c r="A59" s="7"/>
+    </row>
+    <row r="60" ht="18.75" spans="1:1">
+      <c r="A60" s="7"/>
+    </row>
+    <row r="61" ht="18.75" spans="1:1">
+      <c r="A61" s="7"/>
+    </row>
+    <row r="62" ht="18.75" spans="1:1">
+      <c r="A62" s="7"/>
+    </row>
+    <row r="63" ht="18.75" spans="1:1">
+      <c r="A63" s="7"/>
+    </row>
+    <row r="64" ht="18.75" spans="1:1">
+      <c r="A64" s="7"/>
+    </row>
+  </sheetData>
+  <mergeCells count="11">
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A23:C23"/>
+    <mergeCell ref="A3:A21"/>
+    <mergeCell ref="A24:A36"/>
+    <mergeCell ref="B5:B8"/>
+    <mergeCell ref="B10:B19"/>
+    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="B24:B26"/>
+    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="B31:B33"/>
+    <mergeCell ref="B35:B36"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection/>
       <selection pane="bottomLeft" activeCell="E1" sqref="E$1:E$1048576"/>
     </sheetView>
@@ -5999,19 +6495,19 @@
     </row>
     <row r="2" ht="15" spans="1:5">
       <c r="A2" s="2" t="s">
-        <v>370</v>
+        <v>401</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>371</v>
+        <v>402</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>372</v>
+        <v>403</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>373</v>
+        <v>404</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>374</v>
+        <v>405</v>
       </c>
     </row>
     <row r="4" ht="25.5" spans="1:5">
@@ -6019,16 +6515,16 @@
         <v>1</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>375</v>
+        <v>406</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>376</v>
+        <v>407</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>68</v>
       </c>
       <c r="E4" t="s">
-        <v>377</v>
+        <v>408</v>
       </c>
     </row>
     <row r="6" ht="25.5" spans="1:5">
@@ -6036,16 +6532,16 @@
         <v>2</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>378</v>
+        <v>409</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>379</v>
+        <v>410</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>193</v>
       </c>
       <c r="E6" t="s">
-        <v>377</v>
+        <v>408</v>
       </c>
     </row>
     <row r="8" ht="25.5" spans="1:5">
@@ -6053,16 +6549,16 @@
         <v>3</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>380</v>
+        <v>411</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>381</v>
+        <v>412</v>
       </c>
       <c r="D8" s="5" t="s">
         <v>321</v>
       </c>
       <c r="E8" t="s">
-        <v>377</v>
+        <v>408</v>
       </c>
     </row>
   </sheetData>

</xml_diff>